<commit_message>
GISTEMP .xls updated through 2024
</commit_message>
<xml_diff>
--- a/GISTEMP_Arctic_Global_SurfaceTemperature_1880-2021_withLongwaveRadiation.xlsx
+++ b/GISTEMP_Arctic_Global_SurfaceTemperature_1880-2021_withLongwaveRadiation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jen/Documents/jenkay/jek_proposals/2016_NSF_CAREER/Curriculum/v2_data_through2021/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeka1927/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0A6459-7EC8-C54D-9C87-D75801B13E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC500A-6432-EE4E-8F08-BD9B39390170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="460" windowWidth="23240" windowHeight="24880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="500" windowWidth="30700" windowHeight="25260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LWgraph" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -44,9 +49,6 @@
     <t xml:space="preserve"> Hansen et al. 2010; anomaly calculated with respect to 1951-1980 base period </t>
   </si>
   <si>
-    <t xml:space="preserve">Data were downloaded April 2019 from http://www.esrl.noaa.gov/psd/data/gridded/data.gistemp.html </t>
-  </si>
-  <si>
     <t>Global mean temperature (1951-1980) in deg C</t>
   </si>
   <si>
@@ -54,9 +56,6 @@
   </si>
   <si>
     <t>Global blackbody longwave radiation emitted (Wm-2)</t>
-  </si>
-  <si>
-    <t>Data munged by Jennifer.E.Kay@colorado.edu using GISTEMP_timeseries_through2021.ncl</t>
   </si>
   <si>
     <t xml:space="preserve"> last update March 2022 </t>
@@ -69,6 +68,12 @@
   </si>
   <si>
     <t>Arctic mean temperature (estimate) in deg C</t>
+  </si>
+  <si>
+    <t>Data munged by Jennifer.E.Kay@colorado.edu using GISTEMP_timeseries_through2024.ncl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data were downloaded May 2024 from http://www.esrl.noaa.gov/psd/data/gridded/data.gistemp.html </t>
   </si>
 </sst>
 </file>
@@ -762,10 +767,10 @@
                   <c:v>388.78075439053333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>388.29460126362119</c:v>
+                  <c:v>388.3485957501664</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>389.05103663654262</c:v>
+                  <c:v>389.10510999237562</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>388.8888503838723</c:v>
@@ -780,7 +785,7 @@
                   <c:v>388.99696891677559</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>389.32145978420073</c:v>
+                  <c:v>389.37556132623837</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>388.72671484522147</c:v>
@@ -792,7 +797,7 @@
                   <c:v>389.10510999237562</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>389.42966850669217</c:v>
+                  <c:v>389.48378132595394</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>390.24195308984537</c:v>
@@ -807,10 +812,10 @@
                   <c:v>390.02521973919369</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>390.67569076114364</c:v>
+                  <c:v>390.72993338113662</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>390.94696034716645</c:v>
+                  <c:v>390.89269513196621</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>390.02521973919369</c:v>
@@ -939,64 +944,64 @@
                   <c:v>320.56508163200465</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>321.54821192283077</c:v>
+                  <c:v>321.50134498364474</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>321.87642398565549</c:v>
+                  <c:v>321.92333192604372</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>317.1186773501102</c:v>
+                  <c:v>317.16506431349643</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>325.26692216598116</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>325.07786158483344</c:v>
+                  <c:v>325.12511900135144</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>326.21346236396727</c:v>
+                  <c:v>325.97663389858718</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>323.47417234698594</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>323.38002283954052</c:v>
+                  <c:v>323.42709502386759</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>327.11458761176817</c:v>
+                  <c:v>327.30453583213392</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>328.16032673200743</c:v>
+                  <c:v>328.0175785086895</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>328.44596294771134</c:v>
+                  <c:v>328.0175785086895</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>323.23883711556692</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>325.88193862809806</c:v>
+                  <c:v>325.97663389858718</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>325.78726399063476</c:v>
+                  <c:v>325.92928368402693</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>332.84911152955391</c:v>
+                  <c:v>332.80101455345243</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>328.25551809487763</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>326.82982031380078</c:v>
+                  <c:v>326.92472207944598</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>328.92243762799313</c:v>
+                  <c:v>329.25627822655298</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>330.4028041367705</c:v>
+                  <c:v>330.16369803388989</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>326.92472207944598</c:v>
+                  <c:v>327.06711347762115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1247,6 +1252,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1254,7 +1260,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1782,40 +1787,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="142"/>
                 <c:pt idx="0">
-                  <c:v>384.47536115961219</c:v>
+                  <c:v>384.36818659357857</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>384.85064865020979</c:v>
+                  <c:v>384.74339563096243</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>384.68977752870001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>384.36818659357857</c:v>
+                  <c:v>384.31460771382257</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>383.77912694277103</c:v>
+                  <c:v>383.72560965972832</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>383.51159649724525</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>383.67209797404479</c:v>
+                  <c:v>383.61859188532998</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>383.40462349235258</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>384.36818659357857</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>384.79701933800214</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>383.4581071970951</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>384.42177107537833</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>384.85064865020979</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>383.51159649724525</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>384.26103443571941</c:v>
+                  <c:v>384.2074667588796</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>383.83264982356309</c:v>
@@ -1824,91 +1829,91 @@
                   <c:v>383.72560965972832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>383.77912694277103</c:v>
+                  <c:v>383.72560965972832</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>384.15390468291196</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>384.63616503082426</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>384.74339563096243</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>383.83264982356309</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>384.36818659357857</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>384.90428356797594</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>384.52895684667084</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>383.83264982356309</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>383.35114538262775</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>382.87009410650859</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>383.9932520563392</c:v>
+                </c:pt>
+                <c:pt idx="26">
                   <c:v>384.2074667588796</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>384.68977752870001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>384.79701933800214</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>383.93971237995703</c:v>
-                </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="27">
+                  <c:v>383.24420594666913</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>383.13728888609842</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>382.76325533521504</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>383.0303941977939</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>383.0303941977939</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>383.4581071970951</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>383.4581071970951</c:v>
+                </c:pt>
+                <c:pt idx="34">
                   <c:v>384.47536115961219</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>384.95792409169127</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>384.58255813694461</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>383.8861783024949</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>383.40462349235258</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>382.97695524226617</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>384.0467973320321</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>384.26103443571941</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>383.29767286753008</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>383.19074461965545</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>382.87009410650859</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>383.13728888609842</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>383.08383874560803</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>383.51159649724525</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>383.56509139319331</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>384.58255813694461</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>384.63616503082426</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>383.51159649724525</c:v>
+                  <c:v>383.40462349235258</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>382.87009410650859</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>383.77912694277103</c:v>
+                  <c:v>383.72560965972832</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>383.8861783024949</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>383.93971237995703</c:v>
+                  <c:v>383.8861783024949</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>384.42177107537833</c:v>
+                  <c:v>384.36818659357857</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>383.8861783024949</c:v>
+                  <c:v>383.83264982356309</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>383.9932520563392</c:v>
@@ -1917,13 +1922,13 @@
                   <c:v>383.9932520563392</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>384.26103443571941</c:v>
+                  <c:v>384.2074667588796</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>384.90428356797594</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>384.31460771382257</c:v>
+                  <c:v>384.26103443571941</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>384.36818659357857</c:v>
@@ -1941,37 +1946,37 @@
                   <c:v>384.63616503082426</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>383.93971237995703</c:v>
+                  <c:v>383.8861783024949</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>384.79701933800214</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>384.42177107537833</c:v>
+                  <c:v>384.36818659357857</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>384.74339563096243</c:v>
+                  <c:v>384.68977752870001</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>385.38725014245563</c:v>
+                  <c:v>385.33356475708479</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>385.44094113729142</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>385.38725014245563</c:v>
+                  <c:v>385.33356475708479</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>386.1932042776611</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>386.51593962350103</c:v>
+                  <c:v>386.46213635729197</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>385.81693519898806</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>385.97815969219738</c:v>
+                  <c:v>385.92441258121801</c:v>
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>386.51593962350103</c:v>
@@ -1992,10 +1997,10 @@
                   <c:v>384.85064865020979</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>384.52895684667084</c:v>
+                  <c:v>384.47536115961219</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>385.11887930243745</c:v>
+                  <c:v>385.06522195853137</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>385.49463774198318</c:v>
@@ -2019,7 +2024,7 @@
                   <c:v>385.7632049269555</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>385.60204778249698</c:v>
+                  <c:v>385.54833995692138</c:v>
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>385.27988498078827</c:v>
@@ -2055,7 +2060,7 @@
                   <c:v>385.54833995692138</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>384.95792409169127</c:v>
+                  <c:v>385.01157022174618</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>385.44094113729142</c:v>
@@ -2076,7 +2081,7 @@
                   <c:v>386.40833870836519</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>385.81693519898806</c:v>
+                  <c:v>385.7632049269555</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>386.30076026079456</c:v>
@@ -2106,7 +2111,7 @@
                   <c:v>387.10814640427151</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>387.48535941635276</c:v>
+                  <c:v>387.5392694852323</c:v>
                 </c:pt>
                 <c:pt idx="109">
                   <c:v>386.89271980371592</c:v>
@@ -2154,10 +2159,10 @@
                   <c:v>388.78075439053333</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>388.29460126362119</c:v>
+                  <c:v>388.3485957501664</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>389.05103663654262</c:v>
+                  <c:v>389.10510999237562</c:v>
                 </c:pt>
                 <c:pt idx="126">
                   <c:v>388.8888503838723</c:v>
@@ -2172,7 +2177,7 @@
                   <c:v>388.99696891677559</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>389.32145978420073</c:v>
+                  <c:v>389.37556132623837</c:v>
                 </c:pt>
                 <c:pt idx="131">
                   <c:v>388.72671484522147</c:v>
@@ -2184,7 +2189,7 @@
                   <c:v>389.10510999237562</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>389.42966850669217</c:v>
+                  <c:v>389.48378132595394</c:v>
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>390.24195308984537</c:v>
@@ -2199,10 +2204,10 @@
                   <c:v>390.02521973919369</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>390.67569076114364</c:v>
+                  <c:v>390.72993338113662</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>390.94696034716645</c:v>
+                  <c:v>390.89269513196621</c:v>
                 </c:pt>
                 <c:pt idx="141">
                   <c:v>390.02521973919369</c:v>
@@ -2685,25 +2690,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="142"/>
                 <c:pt idx="0">
-                  <c:v>311.04012193891896</c:v>
+                  <c:v>310.94870005051018</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>310.53755092477502</c:v>
+                  <c:v>310.44623985076419</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>307.44425436720354</c:v>
+                  <c:v>307.48957589571449</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>314.85194217859879</c:v>
+                  <c:v>314.9903715939945</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>310.6745553018572</c:v>
+                  <c:v>310.81160500710308</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>306.76503245802877</c:v>
+                  <c:v>306.90078671588617</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>305.36487410804472</c:v>
+                  <c:v>305.40996554885356</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>306.17728436537561</c:v>
@@ -2712,7 +2717,7 @@
                   <c:v>309.12449083844746</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>311.63485568992365</c:v>
+                  <c:v>311.58907668477633</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>310.49189287027872</c:v>
@@ -2721,64 +2726,64 @@
                   <c:v>309.67090851259422</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>309.39760920569358</c:v>
+                  <c:v>309.352076914723</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>312.64327065234374</c:v>
+                  <c:v>312.59738058829214</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>309.76204850418208</c:v>
+                  <c:v>309.5797886342898</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>311.90963566282767</c:v>
+                  <c:v>311.72642883331054</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>310.90299666451727</c:v>
+                  <c:v>310.72023349998278</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>312.82688143621107</c:v>
+                  <c:v>312.68916576879064</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>308.76061433907716</c:v>
+                  <c:v>308.66969543087725</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>309.07898869631936</c:v>
+                  <c:v>309.03349157770413</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>312.13875774794229</c:v>
+                  <c:v>312.09292323576784</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>312.00126935488771</c:v>
+                  <c:v>312.09292323576784</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>308.62424350724052</c:v>
+                  <c:v>307.85232853569312</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>313.6541309743302</c:v>
+                  <c:v>313.51614224722954</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>314.52911764936545</c:v>
+                  <c:v>314.06837046577078</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>314.89808024635863</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>314.34475798539989</c:v>
+                  <c:v>314.29868073564893</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>312.91871714993346</c:v>
+                  <c:v>312.87279676594761</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>314.25260855165118</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>312.04709377153983</c:v>
+                  <c:v>312.00126935488771</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>312.68916576879064</c:v>
+                  <c:v>311.81802215662361</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>313.74614876122854</c:v>
+                  <c:v>313.79216524644022</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>312.55149557626464</c:v>
@@ -2787,100 +2792,100 @@
                   <c:v>312.00126935488771</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>313.33222810823565</c:v>
+                  <c:v>313.28626221931233</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>311.17729256814567</c:v>
+                  <c:v>312.04709377153983</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>313.05650863109679</c:v>
+                  <c:v>312.64327065234374</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>309.48868886630936</c:v>
+                  <c:v>310.44623985076419</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>310.08119690957619</c:v>
+                  <c:v>309.85320861201268</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>311.54330272349921</c:v>
+                  <c:v>312.18459730843387</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>315.22118871776757</c:v>
+                  <c:v>315.03652487461358</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>314.9903715939945</c:v>
+                  <c:v>314.89808024635863</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>313.97628180769811</c:v>
+                  <c:v>314.34475798539989</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>316.70142361426849</c:v>
+                  <c:v>316.8868188521655</c:v>
                 </c:pt>
                 <c:pt idx="44">
+                  <c:v>317.67565685347773</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>315.26736736058308</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>317.7685580538672</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>315.91440125226575</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>319.16452267534032</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>316.8868188521655</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>315.03652487461358</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>317.62921389281217</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>315.86815154587384</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>319.44426659779566</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>316.9795469890347</c:v>
-                </c:pt>
                 <c:pt idx="50">
-                  <c:v>319.11791655729439</c:v>
+                  <c:v>319.02471963415906</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>318.93154312581487</c:v>
+                  <c:v>319.02471963415906</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>318.60558607004424</c:v>
+                  <c:v>318.5125013913663</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>316.05318084547457</c:v>
+                  <c:v>316.1920061575405</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>320.28460181068391</c:v>
+                  <c:v>320.42481870436319</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>317.67565685347773</c:v>
+                  <c:v>317.48991556446401</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>318.3729126194097</c:v>
+                  <c:v>318.5125013913663</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>322.34573414176174</c:v>
+                  <c:v>322.2987800464457</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>324.18094910305086</c:v>
+                  <c:v>324.3696183540489</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>318.46596670161199</c:v>
+                  <c:v>318.41943711108399</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>320.89254087405959</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>315.59075994061396</c:v>
+                  <c:v>315.72943289552609</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>319.95760802314891</c:v>
+                  <c:v>320.05100925822074</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>322.5336018286975</c:v>
+                  <c:v>322.62756646079947</c:v>
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>321.22025092832246</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>319.63086468217966</c:v>
+                  <c:v>319.72419437414351</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>315.91440125226575</c:v>
@@ -2892,43 +2897,43 @@
                   <c:v>315.22118871776757</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>316.56243058048676</c:v>
+                  <c:v>316.51610973765031</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>317.1186773501102</c:v>
+                  <c:v>317.02591868825147</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>315.86815154587384</c:v>
+                  <c:v>315.82190691786786</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>317.86147962881603</c:v>
+                  <c:v>317.90794805768098</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>320.79895550313137</c:v>
+                  <c:v>320.89254087405959</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>320.51832220728426</c:v>
+                  <c:v>320.47156789819479</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>314.85194217859879</c:v>
+                  <c:v>314.89808024635863</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>316.93318037713016</c:v>
+                  <c:v>316.9795469890347</c:v>
                 </c:pt>
                 <c:pt idx="77">
                   <c:v>315.96065603741522</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>315.17501514813443</c:v>
+                  <c:v>315.08268322692891</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>318.18686563380078</c:v>
+                  <c:v>318.2333697337848</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>317.30425573794872</c:v>
+                  <c:v>317.35066305877109</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>314.62132788552441</c:v>
+                  <c:v>314.57522023345405</c:v>
                 </c:pt>
                 <c:pt idx="82">
                   <c:v>317.07229547515254</c:v>
@@ -2937,7 +2942,7 @@
                   <c:v>313.56213342965839</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>312.23044191761312</c:v>
+                  <c:v>312.32214628351784</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>314.80580918104931</c:v>
@@ -2952,37 +2957,37 @@
                   <c:v>313.28626221931233</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>315.86815154587384</c:v>
+                  <c:v>315.91440125226575</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>314.29868073564893</c:v>
+                  <c:v>314.39084030127572</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>315.3597398672477</c:v>
+                  <c:v>315.40593373183998</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>314.89808024635863</c:v>
+                  <c:v>314.85194217859879</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>315.31355107695254</c:v>
+                  <c:v>315.22118871776757</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>315.03652487461358</c:v>
+                  <c:v>315.08268322692891</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>315.22118871776757</c:v>
+                  <c:v>315.26736736058308</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>315.63697918226694</c:v>
+                  <c:v>315.59075994061396</c:v>
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>315.68320350044701</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>314.25260855165118</c:v>
+                  <c:v>314.20654143303597</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>312.13875774794229</c:v>
+                  <c:v>312.04709377153983</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>316.28458176990767</c:v>
@@ -2997,7 +3002,7 @@
                   <c:v>315.91440125226575</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>318.14036663080833</c:v>
+                  <c:v>318.09387272443468</c:v>
                 </c:pt>
                 <c:pt idx="105">
                   <c:v>317.81501629433546</c:v>
@@ -3006,7 +3011,7 @@
                   <c:v>314.89808024635863</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>313.24030138797718</c:v>
+                  <c:v>313.19434561385918</c:v>
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>317.30425573794872</c:v>
@@ -3036,13 +3041,13 @@
                   <c:v>319.58420749919998</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>318.46596670161199</c:v>
+                  <c:v>318.5125013913663</c:v>
                 </c:pt>
                 <c:pt idx="118">
                   <c:v>320.0043060849211</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>317.62921389281217</c:v>
+                  <c:v>317.5827760246695</c:v>
                 </c:pt>
                 <c:pt idx="120">
                   <c:v>319.86422723269442</c:v>
@@ -3051,64 +3056,64 @@
                   <c:v>320.56508163200465</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>321.54821192283077</c:v>
+                  <c:v>321.50134498364474</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>321.87642398565549</c:v>
+                  <c:v>321.92333192604372</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>317.1186773501102</c:v>
+                  <c:v>317.16506431349643</c:v>
                 </c:pt>
                 <c:pt idx="125">
                   <c:v>325.26692216598116</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>325.07786158483344</c:v>
+                  <c:v>325.12511900135144</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>326.21346236396727</c:v>
+                  <c:v>325.97663389858718</c:v>
                 </c:pt>
                 <c:pt idx="128">
                   <c:v>323.47417234698594</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>323.38002283954052</c:v>
+                  <c:v>323.42709502386759</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>327.11458761176817</c:v>
+                  <c:v>327.30453583213392</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>328.16032673200743</c:v>
+                  <c:v>328.0175785086895</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>328.44596294771134</c:v>
+                  <c:v>328.0175785086895</c:v>
                 </c:pt>
                 <c:pt idx="133">
                   <c:v>323.23883711556692</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>325.88193862809806</c:v>
+                  <c:v>325.97663389858718</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>325.78726399063476</c:v>
+                  <c:v>325.92928368402693</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>332.84911152955391</c:v>
+                  <c:v>332.80101455345243</c:v>
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>328.25551809487763</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>326.82982031380078</c:v>
+                  <c:v>326.92472207944598</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>328.92243762799313</c:v>
+                  <c:v>329.25627822655298</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>330.4028041367705</c:v>
+                  <c:v>330.16369803388989</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>326.92472207944598</c:v>
+                  <c:v>327.06711347762115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3359,6 +3364,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3366,7 +3372,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4512,7 +4517,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="168" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4523,7 +4528,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1904E8C6-5EA8-F24D-9F1F-2EE48A32A0CE}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="168" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4534,7 +4539,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670774" cy="6281964"/>
+    <xdr:ext cx="8676298" cy="6288942"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4567,7 +4572,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8676913" cy="6281812"/>
+    <xdr:ext cx="8670774" cy="6281964"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4597,9 +4602,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4637,7 +4642,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4743,7 +4748,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4885,7 +4890,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4893,10 +4898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E150"/>
+  <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4909,7 +4914,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E1">
         <v>14</v>
@@ -4920,7 +4925,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -4941,15 +4946,15 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4959,16 +4964,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -4976,18 +4981,18 @@
         <v>1880</v>
       </c>
       <c r="B9">
-        <v>-0.18</v>
+        <v>-0.2</v>
       </c>
       <c r="C9">
-        <v>-0.99</v>
+        <v>-1.01</v>
       </c>
       <c r="D9">
-        <f>5.67*10^-8*(B9+$E$1+273.14)^4</f>
-        <v>384.47536115961219</v>
+        <f t="shared" ref="D9:D40" si="0">5.67*10^-8*(B9+$E$1+273.14)^4</f>
+        <v>384.36818659357857</v>
       </c>
       <c r="E9">
-        <f>5.67*10^-8*(C9+$E$2+273.14)^4</f>
-        <v>311.04012193891896</v>
+        <f t="shared" ref="E9:E40" si="1">5.67*10^-8*(C9+$E$2+273.14)^4</f>
+        <v>310.94870005051018</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -4995,18 +5000,18 @@
         <v>1881</v>
       </c>
       <c r="B10">
-        <v>-0.11</v>
+        <v>-0.13</v>
       </c>
       <c r="C10">
-        <v>-1.1000000000000001</v>
+        <v>-1.1200000000000001</v>
       </c>
       <c r="D10">
-        <f>5.67*10^-8*(B10+$E$1+273.14)^4</f>
-        <v>384.85064865020979</v>
+        <f t="shared" si="0"/>
+        <v>384.74339563096243</v>
       </c>
       <c r="E10">
-        <f>5.67*10^-8*(C10+$E$2+273.14)^4</f>
-        <v>310.53755092477502</v>
+        <f t="shared" si="1"/>
+        <v>310.44623985076419</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -5017,15 +5022,15 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C11">
-        <v>-1.78</v>
+        <v>-1.77</v>
       </c>
       <c r="D11">
-        <f>5.67*10^-8*(B11+$E$1+273.14)^4</f>
+        <f t="shared" si="0"/>
         <v>384.68977752870001</v>
       </c>
       <c r="E11">
-        <f>5.67*10^-8*(C11+$E$2+273.14)^4</f>
-        <v>307.44425436720354</v>
+        <f t="shared" si="1"/>
+        <v>307.48957589571449</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5033,18 +5038,18 @@
         <v>1883</v>
       </c>
       <c r="B12">
-        <v>-0.2</v>
+        <v>-0.21</v>
       </c>
       <c r="C12">
-        <v>-0.16</v>
+        <v>-0.13</v>
       </c>
       <c r="D12">
-        <f>5.67*10^-8*(B12+$E$1+273.14)^4</f>
-        <v>384.36818659357857</v>
+        <f t="shared" si="0"/>
+        <v>384.31460771382257</v>
       </c>
       <c r="E12">
-        <f>5.67*10^-8*(C12+$E$2+273.14)^4</f>
-        <v>314.85194217859879</v>
+        <f t="shared" si="1"/>
+        <v>314.9903715939945</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -5052,18 +5057,18 @@
         <v>1884</v>
       </c>
       <c r="B13">
-        <v>-0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="C13">
-        <v>-1.07</v>
+        <v>-1.04</v>
       </c>
       <c r="D13">
-        <f>5.67*10^-8*(B13+$E$1+273.14)^4</f>
-        <v>383.77912694277103</v>
+        <f t="shared" si="0"/>
+        <v>383.72560965972832</v>
       </c>
       <c r="E13">
-        <f>5.67*10^-8*(C13+$E$2+273.14)^4</f>
-        <v>310.6745553018572</v>
+        <f t="shared" si="1"/>
+        <v>310.81160500710308</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -5074,15 +5079,15 @@
         <v>-0.36</v>
       </c>
       <c r="C14">
-        <v>-1.93</v>
+        <v>-1.9</v>
       </c>
       <c r="D14">
-        <f>5.67*10^-8*(B14+$E$1+273.14)^4</f>
+        <f t="shared" si="0"/>
         <v>383.51159649724525</v>
       </c>
       <c r="E14">
-        <f>5.67*10^-8*(C14+$E$2+273.14)^4</f>
-        <v>306.76503245802877</v>
+        <f t="shared" si="1"/>
+        <v>306.90078671588617</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5090,18 +5095,18 @@
         <v>1886</v>
       </c>
       <c r="B15">
-        <v>-0.33</v>
+        <v>-0.34</v>
       </c>
       <c r="C15">
-        <v>-2.2400000000000002</v>
+        <v>-2.23</v>
       </c>
       <c r="D15">
-        <f>5.67*10^-8*(B15+$E$1+273.14)^4</f>
-        <v>383.67209797404479</v>
+        <f t="shared" si="0"/>
+        <v>383.61859188532998</v>
       </c>
       <c r="E15">
-        <f>5.67*10^-8*(C15+$E$2+273.14)^4</f>
-        <v>305.36487410804472</v>
+        <f t="shared" si="1"/>
+        <v>305.40996554885356</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -5109,17 +5114,17 @@
         <v>1887</v>
       </c>
       <c r="B16">
-        <v>-0.37</v>
+        <v>-0.38</v>
       </c>
       <c r="C16">
         <v>-2.06</v>
       </c>
       <c r="D16">
-        <f>5.67*10^-8*(B16+$E$1+273.14)^4</f>
-        <v>383.4581071970951</v>
+        <f t="shared" si="0"/>
+        <v>383.40462349235258</v>
       </c>
       <c r="E16">
-        <f>5.67*10^-8*(C16+$E$2+273.14)^4</f>
+        <f t="shared" si="1"/>
         <v>306.17728436537561</v>
       </c>
     </row>
@@ -5128,17 +5133,17 @@
         <v>1888</v>
       </c>
       <c r="B17">
-        <v>-0.19</v>
+        <v>-0.2</v>
       </c>
       <c r="C17">
         <v>-1.41</v>
       </c>
       <c r="D17">
-        <f>5.67*10^-8*(B17+$E$1+273.14)^4</f>
-        <v>384.42177107537833</v>
+        <f t="shared" si="0"/>
+        <v>384.36818659357857</v>
       </c>
       <c r="E17">
-        <f>5.67*10^-8*(C17+$E$2+273.14)^4</f>
+        <f t="shared" si="1"/>
         <v>309.12449083844746</v>
       </c>
     </row>
@@ -5147,18 +5152,18 @@
         <v>1889</v>
       </c>
       <c r="B18">
-        <v>-0.11</v>
+        <v>-0.12</v>
       </c>
       <c r="C18">
-        <v>-0.86</v>
+        <v>-0.87</v>
       </c>
       <c r="D18">
-        <f>5.67*10^-8*(B18+$E$1+273.14)^4</f>
-        <v>384.85064865020979</v>
+        <f t="shared" si="0"/>
+        <v>384.79701933800214</v>
       </c>
       <c r="E18">
-        <f>5.67*10^-8*(C18+$E$2+273.14)^4</f>
-        <v>311.63485568992365</v>
+        <f t="shared" si="1"/>
+        <v>311.58907668477633</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -5166,17 +5171,17 @@
         <v>1890</v>
       </c>
       <c r="B19">
-        <v>-0.36</v>
+        <v>-0.37</v>
       </c>
       <c r="C19">
         <v>-1.1100000000000001</v>
       </c>
       <c r="D19">
-        <f>5.67*10^-8*(B19+$E$1+273.14)^4</f>
-        <v>383.51159649724525</v>
+        <f t="shared" si="0"/>
+        <v>383.4581071970951</v>
       </c>
       <c r="E19">
-        <f>5.67*10^-8*(C19+$E$2+273.14)^4</f>
+        <f t="shared" si="1"/>
         <v>310.49189287027872</v>
       </c>
     </row>
@@ -5185,17 +5190,17 @@
         <v>1891</v>
       </c>
       <c r="B20">
-        <v>-0.22</v>
+        <v>-0.23</v>
       </c>
       <c r="C20">
         <v>-1.29</v>
       </c>
       <c r="D20">
-        <f>5.67*10^-8*(B20+$E$1+273.14)^4</f>
-        <v>384.26103443571941</v>
+        <f t="shared" si="0"/>
+        <v>384.2074667588796</v>
       </c>
       <c r="E20">
-        <f>5.67*10^-8*(C20+$E$2+273.14)^4</f>
+        <f t="shared" si="1"/>
         <v>309.67090851259422</v>
       </c>
     </row>
@@ -5207,15 +5212,15 @@
         <v>-0.3</v>
       </c>
       <c r="C21">
-        <v>-1.35</v>
+        <v>-1.36</v>
       </c>
       <c r="D21">
-        <f>5.67*10^-8*(B21+$E$1+273.14)^4</f>
+        <f t="shared" si="0"/>
         <v>383.83264982356309</v>
       </c>
       <c r="E21">
-        <f>5.67*10^-8*(C21+$E$2+273.14)^4</f>
-        <v>309.39760920569358</v>
+        <f t="shared" si="1"/>
+        <v>309.352076914723</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -5226,15 +5231,15 @@
         <v>-0.32</v>
       </c>
       <c r="C22">
-        <v>-0.64</v>
+        <v>-0.65</v>
       </c>
       <c r="D22">
-        <f>5.67*10^-8*(B22+$E$1+273.14)^4</f>
+        <f t="shared" si="0"/>
         <v>383.72560965972832</v>
       </c>
       <c r="E22">
-        <f>5.67*10^-8*(C22+$E$2+273.14)^4</f>
-        <v>312.64327065234374</v>
+        <f t="shared" si="1"/>
+        <v>312.59738058829214</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -5242,18 +5247,18 @@
         <v>1894</v>
       </c>
       <c r="B23">
-        <v>-0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="C23">
-        <v>-1.27</v>
+        <v>-1.31</v>
       </c>
       <c r="D23">
-        <f>5.67*10^-8*(B23+$E$1+273.14)^4</f>
-        <v>383.77912694277103</v>
+        <f t="shared" si="0"/>
+        <v>383.72560965972832</v>
       </c>
       <c r="E23">
-        <f>5.67*10^-8*(C23+$E$2+273.14)^4</f>
-        <v>309.76204850418208</v>
+        <f t="shared" si="1"/>
+        <v>309.5797886342898</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -5261,18 +5266,18 @@
         <v>1895</v>
       </c>
       <c r="B24">
-        <v>-0.23</v>
+        <v>-0.24</v>
       </c>
       <c r="C24">
-        <v>-0.8</v>
+        <v>-0.84</v>
       </c>
       <c r="D24">
-        <f>5.67*10^-8*(B24+$E$1+273.14)^4</f>
-        <v>384.2074667588796</v>
+        <f t="shared" si="0"/>
+        <v>384.15390468291196</v>
       </c>
       <c r="E24">
-        <f>5.67*10^-8*(C24+$E$2+273.14)^4</f>
-        <v>311.90963566282767</v>
+        <f t="shared" si="1"/>
+        <v>311.72642883331054</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -5280,18 +5285,18 @@
         <v>1896</v>
       </c>
       <c r="B25">
-        <v>-0.14000000000000001</v>
+        <v>-0.15</v>
       </c>
       <c r="C25">
-        <v>-1.02</v>
+        <v>-1.06</v>
       </c>
       <c r="D25">
-        <f>5.67*10^-8*(B25+$E$1+273.14)^4</f>
-        <v>384.68977752870001</v>
+        <f t="shared" si="0"/>
+        <v>384.63616503082426</v>
       </c>
       <c r="E25">
-        <f>5.67*10^-8*(C25+$E$2+273.14)^4</f>
-        <v>310.90299666451727</v>
+        <f t="shared" si="1"/>
+        <v>310.72023349998278</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -5299,18 +5304,18 @@
         <v>1897</v>
       </c>
       <c r="B26">
-        <v>-0.12</v>
+        <v>-0.13</v>
       </c>
       <c r="C26">
-        <v>-0.6</v>
+        <v>-0.63</v>
       </c>
       <c r="D26">
-        <f>5.67*10^-8*(B26+$E$1+273.14)^4</f>
-        <v>384.79701933800214</v>
+        <f t="shared" si="0"/>
+        <v>384.74339563096243</v>
       </c>
       <c r="E26">
-        <f>5.67*10^-8*(C26+$E$2+273.14)^4</f>
-        <v>312.82688143621107</v>
+        <f t="shared" si="1"/>
+        <v>312.68916576879064</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -5318,18 +5323,18 @@
         <v>1898</v>
       </c>
       <c r="B27">
-        <v>-0.28000000000000003</v>
+        <v>-0.3</v>
       </c>
       <c r="C27">
-        <v>-1.49</v>
+        <v>-1.51</v>
       </c>
       <c r="D27">
-        <f>5.67*10^-8*(B27+$E$1+273.14)^4</f>
-        <v>383.93971237995703</v>
+        <f t="shared" si="0"/>
+        <v>383.83264982356309</v>
       </c>
       <c r="E27">
-        <f>5.67*10^-8*(C27+$E$2+273.14)^4</f>
-        <v>308.76061433907716</v>
+        <f t="shared" si="1"/>
+        <v>308.66969543087725</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -5337,18 +5342,18 @@
         <v>1899</v>
       </c>
       <c r="B28">
-        <v>-0.18</v>
+        <v>-0.2</v>
       </c>
       <c r="C28">
-        <v>-1.42</v>
+        <v>-1.43</v>
       </c>
       <c r="D28">
-        <f>5.67*10^-8*(B28+$E$1+273.14)^4</f>
-        <v>384.47536115961219</v>
+        <f t="shared" si="0"/>
+        <v>384.36818659357857</v>
       </c>
       <c r="E28">
-        <f>5.67*10^-8*(C28+$E$2+273.14)^4</f>
-        <v>309.07898869631936</v>
+        <f t="shared" si="1"/>
+        <v>309.03349157770413</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -5356,18 +5361,18 @@
         <v>1900</v>
       </c>
       <c r="B29">
-        <v>-0.09</v>
+        <v>-0.1</v>
       </c>
       <c r="C29">
-        <v>-0.75</v>
+        <v>-0.76</v>
       </c>
       <c r="D29">
-        <f>5.67*10^-8*(B29+$E$1+273.14)^4</f>
-        <v>384.95792409169127</v>
+        <f t="shared" si="0"/>
+        <v>384.90428356797594</v>
       </c>
       <c r="E29">
-        <f>5.67*10^-8*(C29+$E$2+273.14)^4</f>
-        <v>312.13875774794229</v>
+        <f t="shared" si="1"/>
+        <v>312.09292323576784</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -5375,18 +5380,18 @@
         <v>1901</v>
       </c>
       <c r="B30">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="C30">
-        <v>-0.78</v>
+        <v>-0.76</v>
       </c>
       <c r="D30">
-        <f>5.67*10^-8*(B30+$E$1+273.14)^4</f>
-        <v>384.58255813694461</v>
+        <f t="shared" si="0"/>
+        <v>384.52895684667084</v>
       </c>
       <c r="E30">
-        <f>5.67*10^-8*(C30+$E$2+273.14)^4</f>
-        <v>312.00126935488771</v>
+        <f t="shared" si="1"/>
+        <v>312.09292323576784</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -5394,18 +5399,18 @@
         <v>1902</v>
       </c>
       <c r="B31">
-        <v>-0.28999999999999998</v>
+        <v>-0.3</v>
       </c>
       <c r="C31">
-        <v>-1.52</v>
+        <v>-1.69</v>
       </c>
       <c r="D31">
-        <f>5.67*10^-8*(B31+$E$1+273.14)^4</f>
-        <v>383.8861783024949</v>
+        <f t="shared" si="0"/>
+        <v>383.83264982356309</v>
       </c>
       <c r="E31">
-        <f>5.67*10^-8*(C31+$E$2+273.14)^4</f>
-        <v>308.62424350724052</v>
+        <f t="shared" si="1"/>
+        <v>307.85232853569312</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -5413,18 +5418,18 @@
         <v>1903</v>
       </c>
       <c r="B32">
-        <v>-0.38</v>
+        <v>-0.39</v>
       </c>
       <c r="C32">
-        <v>-0.42</v>
+        <v>-0.45</v>
       </c>
       <c r="D32">
-        <f>5.67*10^-8*(B32+$E$1+273.14)^4</f>
-        <v>383.40462349235258</v>
+        <f t="shared" si="0"/>
+        <v>383.35114538262775</v>
       </c>
       <c r="E32">
-        <f>5.67*10^-8*(C32+$E$2+273.14)^4</f>
-        <v>313.6541309743302</v>
+        <f t="shared" si="1"/>
+        <v>313.51614224722954</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -5432,18 +5437,18 @@
         <v>1904</v>
       </c>
       <c r="B33">
-        <v>-0.46</v>
+        <v>-0.48</v>
       </c>
       <c r="C33">
-        <v>-0.23</v>
+        <v>-0.33</v>
       </c>
       <c r="D33">
-        <f>5.67*10^-8*(B33+$E$1+273.14)^4</f>
-        <v>382.97695524226617</v>
+        <f t="shared" si="0"/>
+        <v>382.87009410650859</v>
       </c>
       <c r="E33">
-        <f>5.67*10^-8*(C33+$E$2+273.14)^4</f>
-        <v>314.52911764936545</v>
+        <f t="shared" si="1"/>
+        <v>314.06837046577078</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -5451,17 +5456,17 @@
         <v>1905</v>
       </c>
       <c r="B34">
-        <v>-0.26</v>
+        <v>-0.27</v>
       </c>
       <c r="C34">
         <v>-0.15</v>
       </c>
       <c r="D34">
-        <f>5.67*10^-8*(B34+$E$1+273.14)^4</f>
-        <v>384.0467973320321</v>
+        <f t="shared" si="0"/>
+        <v>383.9932520563392</v>
       </c>
       <c r="E34">
-        <f>5.67*10^-8*(C34+$E$2+273.14)^4</f>
+        <f t="shared" si="1"/>
         <v>314.89808024635863</v>
       </c>
     </row>
@@ -5470,18 +5475,18 @@
         <v>1906</v>
       </c>
       <c r="B35">
-        <v>-0.22</v>
+        <v>-0.23</v>
       </c>
       <c r="C35">
-        <v>-0.27</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="D35">
-        <f>5.67*10^-8*(B35+$E$1+273.14)^4</f>
-        <v>384.26103443571941</v>
+        <f t="shared" si="0"/>
+        <v>384.2074667588796</v>
       </c>
       <c r="E35">
-        <f>5.67*10^-8*(C35+$E$2+273.14)^4</f>
-        <v>314.34475798539989</v>
+        <f t="shared" si="1"/>
+        <v>314.29868073564893</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -5489,18 +5494,18 @@
         <v>1907</v>
       </c>
       <c r="B36">
-        <v>-0.4</v>
+        <v>-0.41</v>
       </c>
       <c r="C36">
-        <v>-0.57999999999999996</v>
+        <v>-0.59</v>
       </c>
       <c r="D36">
-        <f>5.67*10^-8*(B36+$E$1+273.14)^4</f>
-        <v>383.29767286753008</v>
+        <f t="shared" si="0"/>
+        <v>383.24420594666913</v>
       </c>
       <c r="E36">
-        <f>5.67*10^-8*(C36+$E$2+273.14)^4</f>
-        <v>312.91871714993346</v>
+        <f t="shared" si="1"/>
+        <v>312.87279676594761</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -5508,17 +5513,17 @@
         <v>1908</v>
       </c>
       <c r="B37">
-        <v>-0.42</v>
+        <v>-0.43</v>
       </c>
       <c r="C37">
         <v>-0.28999999999999998</v>
       </c>
       <c r="D37">
-        <f>5.67*10^-8*(B37+$E$1+273.14)^4</f>
-        <v>383.19074461965545</v>
+        <f t="shared" si="0"/>
+        <v>383.13728888609842</v>
       </c>
       <c r="E37">
-        <f>5.67*10^-8*(C37+$E$2+273.14)^4</f>
+        <f t="shared" si="1"/>
         <v>314.25260855165118</v>
       </c>
     </row>
@@ -5527,18 +5532,18 @@
         <v>1909</v>
       </c>
       <c r="B38">
-        <v>-0.48</v>
+        <v>-0.5</v>
       </c>
       <c r="C38">
-        <v>-0.77</v>
+        <v>-0.78</v>
       </c>
       <c r="D38">
-        <f>5.67*10^-8*(B38+$E$1+273.14)^4</f>
-        <v>382.87009410650859</v>
+        <f t="shared" si="0"/>
+        <v>382.76325533521504</v>
       </c>
       <c r="E38">
-        <f>5.67*10^-8*(C38+$E$2+273.14)^4</f>
-        <v>312.04709377153983</v>
+        <f t="shared" si="1"/>
+        <v>312.00126935488771</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -5546,18 +5551,18 @@
         <v>1910</v>
       </c>
       <c r="B39">
-        <v>-0.43</v>
+        <v>-0.45</v>
       </c>
       <c r="C39">
-        <v>-0.63</v>
+        <v>-0.82</v>
       </c>
       <c r="D39">
-        <f>5.67*10^-8*(B39+$E$1+273.14)^4</f>
-        <v>383.13728888609842</v>
+        <f t="shared" si="0"/>
+        <v>383.0303941977939</v>
       </c>
       <c r="E39">
-        <f>5.67*10^-8*(C39+$E$2+273.14)^4</f>
-        <v>312.68916576879064</v>
+        <f t="shared" si="1"/>
+        <v>311.81802215662361</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -5565,18 +5570,18 @@
         <v>1911</v>
       </c>
       <c r="B40">
-        <v>-0.44</v>
+        <v>-0.45</v>
       </c>
       <c r="C40">
-        <v>-0.4</v>
+        <v>-0.39</v>
       </c>
       <c r="D40">
-        <f>5.67*10^-8*(B40+$E$1+273.14)^4</f>
-        <v>383.08383874560803</v>
+        <f t="shared" si="0"/>
+        <v>383.0303941977939</v>
       </c>
       <c r="E40">
-        <f>5.67*10^-8*(C40+$E$2+273.14)^4</f>
-        <v>313.74614876122854</v>
+        <f t="shared" si="1"/>
+        <v>313.79216524644022</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -5584,17 +5589,17 @@
         <v>1912</v>
       </c>
       <c r="B41">
-        <v>-0.36</v>
+        <v>-0.37</v>
       </c>
       <c r="C41">
         <v>-0.66</v>
       </c>
       <c r="D41">
-        <f>5.67*10^-8*(B41+$E$1+273.14)^4</f>
-        <v>383.51159649724525</v>
+        <f t="shared" ref="D41:D72" si="2">5.67*10^-8*(B41+$E$1+273.14)^4</f>
+        <v>383.4581071970951</v>
       </c>
       <c r="E41">
-        <f>5.67*10^-8*(C41+$E$2+273.14)^4</f>
+        <f t="shared" ref="E41:E72" si="3">5.67*10^-8*(C41+$E$2+273.14)^4</f>
         <v>312.55149557626464</v>
       </c>
     </row>
@@ -5603,17 +5608,17 @@
         <v>1913</v>
       </c>
       <c r="B42">
-        <v>-0.35</v>
+        <v>-0.37</v>
       </c>
       <c r="C42">
         <v>-0.78</v>
       </c>
       <c r="D42">
-        <f>5.67*10^-8*(B42+$E$1+273.14)^4</f>
-        <v>383.56509139319331</v>
+        <f t="shared" si="2"/>
+        <v>383.4581071970951</v>
       </c>
       <c r="E42">
-        <f>5.67*10^-8*(C42+$E$2+273.14)^4</f>
+        <f t="shared" si="3"/>
         <v>312.00126935488771</v>
       </c>
     </row>
@@ -5622,18 +5627,18 @@
         <v>1914</v>
       </c>
       <c r="B43">
-        <v>-0.16</v>
+        <v>-0.18</v>
       </c>
       <c r="C43">
-        <v>-0.49</v>
+        <v>-0.5</v>
       </c>
       <c r="D43">
-        <f>5.67*10^-8*(B43+$E$1+273.14)^4</f>
-        <v>384.58255813694461</v>
+        <f t="shared" si="2"/>
+        <v>384.47536115961219</v>
       </c>
       <c r="E43">
-        <f>5.67*10^-8*(C43+$E$2+273.14)^4</f>
-        <v>313.33222810823565</v>
+        <f t="shared" si="3"/>
+        <v>313.28626221931233</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -5644,15 +5649,15 @@
         <v>-0.15</v>
       </c>
       <c r="C44">
-        <v>-0.96</v>
+        <v>-0.77</v>
       </c>
       <c r="D44">
-        <f>5.67*10^-8*(B44+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>384.63616503082426</v>
       </c>
       <c r="E44">
-        <f>5.67*10^-8*(C44+$E$2+273.14)^4</f>
-        <v>311.17729256814567</v>
+        <f t="shared" si="3"/>
+        <v>312.04709377153983</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -5660,18 +5665,18 @@
         <v>1916</v>
       </c>
       <c r="B45">
-        <v>-0.36</v>
+        <v>-0.38</v>
       </c>
       <c r="C45">
-        <v>-0.55000000000000004</v>
+        <v>-0.64</v>
       </c>
       <c r="D45">
-        <f>5.67*10^-8*(B45+$E$1+273.14)^4</f>
-        <v>383.51159649724525</v>
+        <f t="shared" si="2"/>
+        <v>383.40462349235258</v>
       </c>
       <c r="E45">
-        <f>5.67*10^-8*(C45+$E$2+273.14)^4</f>
-        <v>313.05650863109679</v>
+        <f t="shared" si="3"/>
+        <v>312.64327065234374</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -5682,15 +5687,15 @@
         <v>-0.48</v>
       </c>
       <c r="C46">
-        <v>-1.33</v>
+        <v>-1.1200000000000001</v>
       </c>
       <c r="D46">
-        <f>5.67*10^-8*(B46+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>382.87009410650859</v>
       </c>
       <c r="E46">
-        <f>5.67*10^-8*(C46+$E$2+273.14)^4</f>
-        <v>309.48868886630936</v>
+        <f t="shared" si="3"/>
+        <v>310.44623985076419</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -5698,18 +5703,18 @@
         <v>1918</v>
       </c>
       <c r="B47">
-        <v>-0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="C47">
-        <v>-1.2</v>
+        <v>-1.25</v>
       </c>
       <c r="D47">
-        <f>5.67*10^-8*(B47+$E$1+273.14)^4</f>
-        <v>383.77912694277103</v>
+        <f t="shared" si="2"/>
+        <v>383.72560965972832</v>
       </c>
       <c r="E47">
-        <f>5.67*10^-8*(C47+$E$2+273.14)^4</f>
-        <v>310.08119690957619</v>
+        <f t="shared" si="3"/>
+        <v>309.85320861201268</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -5720,15 +5725,15 @@
         <v>-0.28999999999999998</v>
       </c>
       <c r="C48">
-        <v>-0.88</v>
+        <v>-0.74</v>
       </c>
       <c r="D48">
-        <f>5.67*10^-8*(B48+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>383.8861783024949</v>
       </c>
       <c r="E48">
-        <f>5.67*10^-8*(C48+$E$2+273.14)^4</f>
-        <v>311.54330272349921</v>
+        <f t="shared" si="3"/>
+        <v>312.18459730843387</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -5736,18 +5741,18 @@
         <v>1920</v>
       </c>
       <c r="B49">
-        <v>-0.28000000000000003</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="C49">
-        <v>-0.08</v>
+        <v>-0.12</v>
       </c>
       <c r="D49">
-        <f>5.67*10^-8*(B49+$E$1+273.14)^4</f>
-        <v>383.93971237995703</v>
+        <f t="shared" si="2"/>
+        <v>383.8861783024949</v>
       </c>
       <c r="E49">
-        <f>5.67*10^-8*(C49+$E$2+273.14)^4</f>
-        <v>315.22118871776757</v>
+        <f t="shared" si="3"/>
+        <v>315.03652487461358</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -5755,18 +5760,18 @@
         <v>1921</v>
       </c>
       <c r="B50">
-        <v>-0.19</v>
+        <v>-0.2</v>
       </c>
       <c r="C50">
-        <v>-0.13</v>
+        <v>-0.15</v>
       </c>
       <c r="D50">
-        <f>5.67*10^-8*(B50+$E$1+273.14)^4</f>
-        <v>384.42177107537833</v>
+        <f t="shared" si="2"/>
+        <v>384.36818659357857</v>
       </c>
       <c r="E50">
-        <f>5.67*10^-8*(C50+$E$2+273.14)^4</f>
-        <v>314.9903715939945</v>
+        <f t="shared" si="3"/>
+        <v>314.89808024635863</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -5774,18 +5779,18 @@
         <v>1922</v>
       </c>
       <c r="B51">
-        <v>-0.28999999999999998</v>
+        <v>-0.3</v>
       </c>
       <c r="C51">
-        <v>-0.35</v>
+        <v>-0.27</v>
       </c>
       <c r="D51">
-        <f>5.67*10^-8*(B51+$E$1+273.14)^4</f>
-        <v>383.8861783024949</v>
+        <f t="shared" si="2"/>
+        <v>383.83264982356309</v>
       </c>
       <c r="E51">
-        <f>5.67*10^-8*(C51+$E$2+273.14)^4</f>
-        <v>313.97628180769811</v>
+        <f t="shared" si="3"/>
+        <v>314.34475798539989</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -5796,15 +5801,15 @@
         <v>-0.27</v>
       </c>
       <c r="C52">
-        <v>0.24</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D52">
-        <f>5.67*10^-8*(B52+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>383.9932520563392</v>
       </c>
       <c r="E52">
-        <f>5.67*10^-8*(C52+$E$2+273.14)^4</f>
-        <v>316.70142361426849</v>
+        <f t="shared" si="3"/>
+        <v>316.8868188521655</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -5815,15 +5820,15 @@
         <v>-0.27</v>
       </c>
       <c r="C53">
-        <v>0.28000000000000003</v>
+        <v>0.45</v>
       </c>
       <c r="D53">
-        <f>5.67*10^-8*(B53+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>383.9932520563392</v>
       </c>
       <c r="E53">
-        <f>5.67*10^-8*(C53+$E$2+273.14)^4</f>
-        <v>316.8868188521655</v>
+        <f t="shared" si="3"/>
+        <v>317.67565685347773</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -5831,18 +5836,18 @@
         <v>1925</v>
       </c>
       <c r="B54">
-        <v>-0.22</v>
+        <v>-0.23</v>
       </c>
       <c r="C54">
-        <v>-0.12</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D54">
-        <f>5.67*10^-8*(B54+$E$1+273.14)^4</f>
-        <v>384.26103443571941</v>
+        <f t="shared" si="2"/>
+        <v>384.2074667588796</v>
       </c>
       <c r="E54">
-        <f>5.67*10^-8*(C54+$E$2+273.14)^4</f>
-        <v>315.03652487461358</v>
+        <f t="shared" si="3"/>
+        <v>315.26736736058308</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -5853,15 +5858,15 @@
         <v>-0.1</v>
       </c>
       <c r="C55">
-        <v>0.44</v>
+        <v>0.47</v>
       </c>
       <c r="D55">
-        <f>5.67*10^-8*(B55+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>384.90428356797594</v>
       </c>
       <c r="E55">
-        <f>5.67*10^-8*(C55+$E$2+273.14)^4</f>
-        <v>317.62921389281217</v>
+        <f t="shared" si="3"/>
+        <v>317.7685580538672</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -5869,18 +5874,18 @@
         <v>1927</v>
       </c>
       <c r="B56">
-        <v>-0.21</v>
+        <v>-0.22</v>
       </c>
       <c r="C56">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D56">
-        <f>5.67*10^-8*(B56+$E$1+273.14)^4</f>
-        <v>384.31460771382257</v>
+        <f t="shared" si="2"/>
+        <v>384.26103443571941</v>
       </c>
       <c r="E56">
-        <f>5.67*10^-8*(C56+$E$2+273.14)^4</f>
-        <v>315.86815154587384</v>
+        <f t="shared" si="3"/>
+        <v>315.91440125226575</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -5891,15 +5896,15 @@
         <v>-0.2</v>
       </c>
       <c r="C57">
-        <v>0.83</v>
+        <v>0.77</v>
       </c>
       <c r="D57">
-        <f>5.67*10^-8*(B57+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>384.36818659357857</v>
       </c>
       <c r="E57">
-        <f>5.67*10^-8*(C57+$E$2+273.14)^4</f>
-        <v>319.44426659779566</v>
+        <f t="shared" si="3"/>
+        <v>319.16452267534032</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -5910,15 +5915,15 @@
         <v>-0.36</v>
       </c>
       <c r="C58">
-        <v>0.3</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D58">
-        <f>5.67*10^-8*(B58+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>383.51159649724525</v>
       </c>
       <c r="E58">
-        <f>5.67*10^-8*(C58+$E$2+273.14)^4</f>
-        <v>316.9795469890347</v>
+        <f t="shared" si="3"/>
+        <v>316.8868188521655</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -5929,15 +5934,15 @@
         <v>-0.15</v>
       </c>
       <c r="C59">
-        <v>0.76</v>
+        <v>0.74</v>
       </c>
       <c r="D59">
-        <f>5.67*10^-8*(B59+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>384.63616503082426</v>
       </c>
       <c r="E59">
-        <f>5.67*10^-8*(C59+$E$2+273.14)^4</f>
-        <v>319.11791655729439</v>
+        <f t="shared" si="3"/>
+        <v>319.02471963415906</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -5948,15 +5953,15 @@
         <v>-0.08</v>
       </c>
       <c r="C60">
-        <v>0.72</v>
+        <v>0.74</v>
       </c>
       <c r="D60">
-        <f>5.67*10^-8*(B60+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>385.01157022174618</v>
       </c>
       <c r="E60">
-        <f>5.67*10^-8*(C60+$E$2+273.14)^4</f>
-        <v>318.93154312581487</v>
+        <f t="shared" si="3"/>
+        <v>319.02471963415906</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -5967,15 +5972,15 @@
         <v>-0.15</v>
       </c>
       <c r="C61">
-        <v>0.65</v>
+        <v>0.63</v>
       </c>
       <c r="D61">
-        <f>5.67*10^-8*(B61+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>384.63616503082426</v>
       </c>
       <c r="E61">
-        <f>5.67*10^-8*(C61+$E$2+273.14)^4</f>
-        <v>318.60558607004424</v>
+        <f t="shared" si="3"/>
+        <v>318.5125013913663</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -5983,18 +5988,18 @@
         <v>1933</v>
       </c>
       <c r="B62">
-        <v>-0.28000000000000003</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="C62">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="D62">
-        <f>5.67*10^-8*(B62+$E$1+273.14)^4</f>
-        <v>383.93971237995703</v>
+        <f t="shared" si="2"/>
+        <v>383.8861783024949</v>
       </c>
       <c r="E62">
-        <f>5.67*10^-8*(C62+$E$2+273.14)^4</f>
-        <v>316.05318084547457</v>
+        <f t="shared" si="3"/>
+        <v>316.1920061575405</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -6005,15 +6010,15 @@
         <v>-0.12</v>
       </c>
       <c r="C63">
-        <v>1.01</v>
+        <v>1.04</v>
       </c>
       <c r="D63">
-        <f>5.67*10^-8*(B63+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>384.79701933800214</v>
       </c>
       <c r="E63">
-        <f>5.67*10^-8*(C63+$E$2+273.14)^4</f>
-        <v>320.28460181068391</v>
+        <f t="shared" si="3"/>
+        <v>320.42481870436319</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -6021,18 +6026,18 @@
         <v>1935</v>
       </c>
       <c r="B64">
-        <v>-0.19</v>
+        <v>-0.2</v>
       </c>
       <c r="C64">
-        <v>0.45</v>
+        <v>0.41</v>
       </c>
       <c r="D64">
-        <f>5.67*10^-8*(B64+$E$1+273.14)^4</f>
-        <v>384.42177107537833</v>
+        <f t="shared" si="2"/>
+        <v>384.36818659357857</v>
       </c>
       <c r="E64">
-        <f>5.67*10^-8*(C64+$E$2+273.14)^4</f>
-        <v>317.67565685347773</v>
+        <f t="shared" si="3"/>
+        <v>317.48991556446401</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -6040,18 +6045,18 @@
         <v>1936</v>
       </c>
       <c r="B65">
-        <v>-0.13</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="C65">
-        <v>0.6</v>
+        <v>0.63</v>
       </c>
       <c r="D65">
-        <f>5.67*10^-8*(B65+$E$1+273.14)^4</f>
-        <v>384.74339563096243</v>
+        <f t="shared" si="2"/>
+        <v>384.68977752870001</v>
       </c>
       <c r="E65">
-        <f>5.67*10^-8*(C65+$E$2+273.14)^4</f>
-        <v>318.3729126194097</v>
+        <f t="shared" si="3"/>
+        <v>318.5125013913663</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -6059,18 +6064,18 @@
         <v>1937</v>
       </c>
       <c r="B66">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="C66">
-        <v>1.45</v>
+        <v>1.44</v>
       </c>
       <c r="D66">
-        <f>5.67*10^-8*(B66+$E$1+273.14)^4</f>
-        <v>385.38725014245563</v>
+        <f t="shared" si="2"/>
+        <v>385.33356475708479</v>
       </c>
       <c r="E66">
-        <f>5.67*10^-8*(C66+$E$2+273.14)^4</f>
-        <v>322.34573414176174</v>
+        <f t="shared" si="3"/>
+        <v>322.2987800464457</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -6081,15 +6086,15 @@
         <v>0</v>
       </c>
       <c r="C67">
-        <v>1.84</v>
+        <v>1.88</v>
       </c>
       <c r="D67">
-        <f>5.67*10^-8*(B67+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>385.44094113729142</v>
       </c>
       <c r="E67">
-        <f>5.67*10^-8*(C67+$E$2+273.14)^4</f>
-        <v>324.18094910305086</v>
+        <f t="shared" si="3"/>
+        <v>324.3696183540489</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -6097,18 +6102,18 @@
         <v>1939</v>
       </c>
       <c r="B68">
-        <v>-0.01</v>
+        <v>-0.02</v>
       </c>
       <c r="C68">
-        <v>0.62</v>
+        <v>0.61</v>
       </c>
       <c r="D68">
-        <f>5.67*10^-8*(B68+$E$1+273.14)^4</f>
-        <v>385.38725014245563</v>
+        <f t="shared" si="2"/>
+        <v>385.33356475708479</v>
       </c>
       <c r="E68">
-        <f>5.67*10^-8*(C68+$E$2+273.14)^4</f>
-        <v>318.46596670161199</v>
+        <f t="shared" si="3"/>
+        <v>318.41943711108399</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -6122,11 +6127,11 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="D69">
-        <f>5.67*10^-8*(B69+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>386.1932042776611</v>
       </c>
       <c r="E69">
-        <f>5.67*10^-8*(C69+$E$2+273.14)^4</f>
+        <f t="shared" si="3"/>
         <v>320.89254087405959</v>
       </c>
     </row>
@@ -6135,18 +6140,18 @@
         <v>1941</v>
       </c>
       <c r="B70">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="D70">
-        <f>5.67*10^-8*(B70+$E$1+273.14)^4</f>
-        <v>386.51593962350103</v>
+        <f t="shared" si="2"/>
+        <v>386.46213635729197</v>
       </c>
       <c r="E70">
-        <f>5.67*10^-8*(C70+$E$2+273.14)^4</f>
-        <v>315.59075994061396</v>
+        <f t="shared" si="3"/>
+        <v>315.72943289552609</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -6157,15 +6162,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C71">
-        <v>0.94</v>
+        <v>0.96</v>
       </c>
       <c r="D71">
-        <f>5.67*10^-8*(B71+$E$1+273.14)^4</f>
+        <f t="shared" si="2"/>
         <v>385.81693519898806</v>
       </c>
       <c r="E71">
-        <f>5.67*10^-8*(C71+$E$2+273.14)^4</f>
-        <v>319.95760802314891</v>
+        <f t="shared" si="3"/>
+        <v>320.05100925822074</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -6173,18 +6178,18 @@
         <v>1943</v>
       </c>
       <c r="B72">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="C72">
-        <v>1.49</v>
+        <v>1.51</v>
       </c>
       <c r="D72">
-        <f>5.67*10^-8*(B72+$E$1+273.14)^4</f>
-        <v>385.97815969219738</v>
+        <f t="shared" si="2"/>
+        <v>385.92441258121801</v>
       </c>
       <c r="E72">
-        <f>5.67*10^-8*(C72+$E$2+273.14)^4</f>
-        <v>322.5336018286975</v>
+        <f t="shared" si="3"/>
+        <v>322.62756646079947</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -6198,11 +6203,11 @@
         <v>1.21</v>
       </c>
       <c r="D73">
-        <f>5.67*10^-8*(B73+$E$1+273.14)^4</f>
+        <f t="shared" ref="D73:D104" si="4">5.67*10^-8*(B73+$E$1+273.14)^4</f>
         <v>386.51593962350103</v>
       </c>
       <c r="E73">
-        <f>5.67*10^-8*(C73+$E$2+273.14)^4</f>
+        <f t="shared" ref="E73:E104" si="5">5.67*10^-8*(C73+$E$2+273.14)^4</f>
         <v>321.22025092832246</v>
       </c>
     </row>
@@ -6214,15 +6219,15 @@
         <v>0.1</v>
       </c>
       <c r="C74">
-        <v>0.87</v>
+        <v>0.89</v>
       </c>
       <c r="D74">
-        <f>5.67*10^-8*(B74+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.97815969219738</v>
       </c>
       <c r="E74">
-        <f>5.67*10^-8*(C74+$E$2+273.14)^4</f>
-        <v>319.63086468217966</v>
+        <f t="shared" si="5"/>
+        <v>319.72419437414351</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -6236,11 +6241,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D75">
-        <f>5.67*10^-8*(B75+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.06522195853137</v>
       </c>
       <c r="E75">
-        <f>5.67*10^-8*(C75+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>315.91440125226575</v>
       </c>
     </row>
@@ -6255,11 +6260,11 @@
         <v>1.34</v>
       </c>
       <c r="D76">
-        <f>5.67*10^-8*(B76+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.38725014245563</v>
       </c>
       <c r="E76">
-        <f>5.67*10^-8*(C76+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>321.82952117172454</v>
       </c>
     </row>
@@ -6274,11 +6279,11 @@
         <v>-0.08</v>
       </c>
       <c r="D77">
-        <f>5.67*10^-8*(B77+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>384.90428356797594</v>
       </c>
       <c r="E77">
-        <f>5.67*10^-8*(C77+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>315.22118871776757</v>
       </c>
     </row>
@@ -6290,15 +6295,15 @@
         <v>-0.11</v>
       </c>
       <c r="C78">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="D78">
-        <f>5.67*10^-8*(B78+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>384.85064865020979</v>
       </c>
       <c r="E78">
-        <f>5.67*10^-8*(C78+$E$2+273.14)^4</f>
-        <v>316.56243058048676</v>
+        <f t="shared" si="5"/>
+        <v>316.51610973765031</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -6306,18 +6311,18 @@
         <v>1950</v>
       </c>
       <c r="B79">
-        <v>-0.17</v>
+        <v>-0.18</v>
       </c>
       <c r="C79">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="D79">
-        <f>5.67*10^-8*(B79+$E$1+273.14)^4</f>
-        <v>384.52895684667084</v>
+        <f t="shared" si="4"/>
+        <v>384.47536115961219</v>
       </c>
       <c r="E79">
-        <f>5.67*10^-8*(C79+$E$2+273.14)^4</f>
-        <v>317.1186773501102</v>
+        <f t="shared" si="5"/>
+        <v>317.02591868825147</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -6325,18 +6330,18 @@
         <v>1951</v>
       </c>
       <c r="B80">
-        <v>-0.06</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="C80">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="D80">
-        <f>5.67*10^-8*(B80+$E$1+273.14)^4</f>
-        <v>385.11887930243745</v>
+        <f t="shared" si="4"/>
+        <v>385.06522195853137</v>
       </c>
       <c r="E80">
-        <f>5.67*10^-8*(C80+$E$2+273.14)^4</f>
-        <v>315.86815154587384</v>
+        <f t="shared" si="5"/>
+        <v>315.82190691786786</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -6347,15 +6352,15 @@
         <v>0.01</v>
       </c>
       <c r="C81">
-        <v>0.49</v>
+        <v>0.5</v>
       </c>
       <c r="D81">
-        <f>5.67*10^-8*(B81+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.49463774198318</v>
       </c>
       <c r="E81">
-        <f>5.67*10^-8*(C81+$E$2+273.14)^4</f>
-        <v>317.86147962881603</v>
+        <f t="shared" si="5"/>
+        <v>317.90794805768098</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -6366,15 +6371,15 @@
         <v>0.09</v>
       </c>
       <c r="C82">
-        <v>1.1200000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D82">
-        <f>5.67*10^-8*(B82+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.92441258121801</v>
       </c>
       <c r="E82">
-        <f>5.67*10^-8*(C82+$E$2+273.14)^4</f>
-        <v>320.79895550313137</v>
+        <f t="shared" si="5"/>
+        <v>320.89254087405959</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -6385,15 +6390,15 @@
         <v>-0.13</v>
       </c>
       <c r="C83">
-        <v>1.06</v>
+        <v>1.05</v>
       </c>
       <c r="D83">
-        <f>5.67*10^-8*(B83+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>384.74339563096243</v>
       </c>
       <c r="E83">
-        <f>5.67*10^-8*(C83+$E$2+273.14)^4</f>
-        <v>320.51832220728426</v>
+        <f t="shared" si="5"/>
+        <v>320.47156789819479</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -6404,15 +6409,15 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C84">
-        <v>-0.16</v>
+        <v>-0.15</v>
       </c>
       <c r="D84">
-        <f>5.67*10^-8*(B84+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>384.68977752870001</v>
       </c>
       <c r="E84">
-        <f>5.67*10^-8*(C84+$E$2+273.14)^4</f>
-        <v>314.85194217859879</v>
+        <f t="shared" si="5"/>
+        <v>314.89808024635863</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -6423,15 +6428,15 @@
         <v>-0.18</v>
       </c>
       <c r="C85">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="D85">
-        <f>5.67*10^-8*(B85+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>384.47536115961219</v>
       </c>
       <c r="E85">
-        <f>5.67*10^-8*(C85+$E$2+273.14)^4</f>
-        <v>316.93318037713016</v>
+        <f t="shared" si="5"/>
+        <v>316.9795469890347</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -6445,11 +6450,11 @@
         <v>0.08</v>
       </c>
       <c r="D86">
-        <f>5.67*10^-8*(B86+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.7094802671233</v>
       </c>
       <c r="E86">
-        <f>5.67*10^-8*(C86+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>315.96065603741522</v>
       </c>
     </row>
@@ -6461,15 +6466,15 @@
         <v>0.06</v>
       </c>
       <c r="C87">
-        <v>-0.09</v>
+        <v>-0.11</v>
       </c>
       <c r="D87">
-        <f>5.67*10^-8*(B87+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.7632049269555</v>
       </c>
       <c r="E87">
-        <f>5.67*10^-8*(C87+$E$2+273.14)^4</f>
-        <v>315.17501514813443</v>
+        <f t="shared" si="5"/>
+        <v>315.08268322692891</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -6477,18 +6482,18 @@
         <v>1959</v>
       </c>
       <c r="B88">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="C88">
-        <v>0.56000000000000005</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="D88">
-        <f>5.67*10^-8*(B88+$E$1+273.14)^4</f>
-        <v>385.60204778249698</v>
+        <f t="shared" si="4"/>
+        <v>385.54833995692138</v>
       </c>
       <c r="E88">
-        <f>5.67*10^-8*(C88+$E$2+273.14)^4</f>
-        <v>318.18686563380078</v>
+        <f t="shared" si="5"/>
+        <v>318.2333697337848</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -6499,15 +6504,15 @@
         <v>-0.03</v>
       </c>
       <c r="C89">
-        <v>0.37</v>
+        <v>0.38</v>
       </c>
       <c r="D89">
-        <f>5.67*10^-8*(B89+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.27988498078827</v>
       </c>
       <c r="E89">
-        <f>5.67*10^-8*(C89+$E$2+273.14)^4</f>
-        <v>317.30425573794872</v>
+        <f t="shared" si="5"/>
+        <v>317.35066305877109</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -6518,15 +6523,15 @@
         <v>0.06</v>
       </c>
       <c r="C90">
-        <v>-0.21</v>
+        <v>-0.22</v>
       </c>
       <c r="D90">
-        <f>5.67*10^-8*(B90+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.7632049269555</v>
       </c>
       <c r="E90">
-        <f>5.67*10^-8*(C90+$E$2+273.14)^4</f>
-        <v>314.62132788552441</v>
+        <f t="shared" si="5"/>
+        <v>314.57522023345405</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -6540,11 +6545,11 @@
         <v>0.32</v>
       </c>
       <c r="D91">
-        <f>5.67*10^-8*(B91+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.60204778249698</v>
       </c>
       <c r="E91">
-        <f>5.67*10^-8*(C91+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>317.07229547515254</v>
       </c>
     </row>
@@ -6559,11 +6564,11 @@
         <v>-0.44</v>
       </c>
       <c r="D92">
-        <f>5.67*10^-8*(B92+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.7632049269555</v>
       </c>
       <c r="E92">
-        <f>5.67*10^-8*(C92+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>313.56213342965839</v>
       </c>
     </row>
@@ -6575,15 +6580,15 @@
         <v>-0.2</v>
       </c>
       <c r="C93">
-        <v>-0.73</v>
+        <v>-0.71</v>
       </c>
       <c r="D93">
-        <f>5.67*10^-8*(B93+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>384.36818659357857</v>
       </c>
       <c r="E93">
-        <f>5.67*10^-8*(C93+$E$2+273.14)^4</f>
-        <v>312.23044191761312</v>
+        <f t="shared" si="5"/>
+        <v>312.32214628351784</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -6597,11 +6602,11 @@
         <v>-0.17</v>
       </c>
       <c r="D94">
-        <f>5.67*10^-8*(B94+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>384.85064865020979</v>
       </c>
       <c r="E94">
-        <f>5.67*10^-8*(C94+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>314.80580918104931</v>
       </c>
     </row>
@@ -6616,11 +6621,11 @@
         <v>-0.78</v>
       </c>
       <c r="D95">
-        <f>5.67*10^-8*(B95+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.11887930243745</v>
       </c>
       <c r="E95">
-        <f>5.67*10^-8*(C95+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>312.00126935488771</v>
       </c>
     </row>
@@ -6635,11 +6640,11 @@
         <v>0.26</v>
       </c>
       <c r="D96">
-        <f>5.67*10^-8*(B96+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.33356475708479</v>
       </c>
       <c r="E96">
-        <f>5.67*10^-8*(C96+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>316.79411106156897</v>
       </c>
     </row>
@@ -6654,11 +6659,11 @@
         <v>-0.5</v>
       </c>
       <c r="D97">
-        <f>5.67*10^-8*(B97+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.01157022174618</v>
       </c>
       <c r="E97">
-        <f>5.67*10^-8*(C97+$E$2+273.14)^4</f>
+        <f t="shared" si="5"/>
         <v>313.28626221931233</v>
       </c>
     </row>
@@ -6670,15 +6675,15 @@
         <v>0.05</v>
       </c>
       <c r="C98">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D98">
-        <f>5.67*10^-8*(B98+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.7094802671233</v>
       </c>
       <c r="E98">
-        <f>5.67*10^-8*(C98+$E$2+273.14)^4</f>
-        <v>315.86815154587384</v>
+        <f t="shared" si="5"/>
+        <v>315.91440125226575</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -6689,15 +6694,15 @@
         <v>0.02</v>
       </c>
       <c r="C99">
-        <v>-0.28000000000000003</v>
+        <v>-0.26</v>
       </c>
       <c r="D99">
-        <f>5.67*10^-8*(B99+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.54833995692138</v>
       </c>
       <c r="E99">
-        <f>5.67*10^-8*(C99+$E$2+273.14)^4</f>
-        <v>314.29868073564893</v>
+        <f t="shared" si="5"/>
+        <v>314.39084030127572</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -6705,18 +6710,18 @@
         <v>1971</v>
       </c>
       <c r="B100">
-        <v>-0.09</v>
+        <v>-0.08</v>
       </c>
       <c r="C100">
-        <v>-0.05</v>
+        <v>-0.04</v>
       </c>
       <c r="D100">
-        <f>5.67*10^-8*(B100+$E$1+273.14)^4</f>
-        <v>384.95792409169127</v>
+        <f t="shared" si="4"/>
+        <v>385.01157022174618</v>
       </c>
       <c r="E100">
-        <f>5.67*10^-8*(C100+$E$2+273.14)^4</f>
-        <v>315.3597398672477</v>
+        <f t="shared" si="5"/>
+        <v>315.40593373183998</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -6727,15 +6732,15 @@
         <v>0</v>
       </c>
       <c r="C101">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="D101">
-        <f>5.67*10^-8*(B101+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.44094113729142</v>
       </c>
       <c r="E101">
-        <f>5.67*10^-8*(C101+$E$2+273.14)^4</f>
-        <v>314.89808024635863</v>
+        <f t="shared" si="5"/>
+        <v>314.85194217859879</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -6746,15 +6751,15 @@
         <v>0.17</v>
       </c>
       <c r="C102">
-        <v>-0.06</v>
+        <v>-0.08</v>
       </c>
       <c r="D102">
-        <f>5.67*10^-8*(B102+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>386.35454667632962</v>
       </c>
       <c r="E102">
-        <f>5.67*10^-8*(C102+$E$2+273.14)^4</f>
-        <v>315.31355107695254</v>
+        <f t="shared" si="5"/>
+        <v>315.22118871776757</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -6765,15 +6770,15 @@
         <v>-0.06</v>
       </c>
       <c r="C103">
-        <v>-0.12</v>
+        <v>-0.11</v>
       </c>
       <c r="D103">
-        <f>5.67*10^-8*(B103+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.11887930243745</v>
       </c>
       <c r="E103">
-        <f>5.67*10^-8*(C103+$E$2+273.14)^4</f>
-        <v>315.03652487461358</v>
+        <f t="shared" si="5"/>
+        <v>315.08268322692891</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -6784,15 +6789,15 @@
         <v>-0.02</v>
       </c>
       <c r="C104">
-        <v>-0.08</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="D104">
-        <f>5.67*10^-8*(B104+$E$1+273.14)^4</f>
+        <f t="shared" si="4"/>
         <v>385.33356475708479</v>
       </c>
       <c r="E104">
-        <f>5.67*10^-8*(C104+$E$2+273.14)^4</f>
-        <v>315.22118871776757</v>
+        <f t="shared" si="5"/>
+        <v>315.26736736058308</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -6803,15 +6808,15 @@
         <v>-0.11</v>
       </c>
       <c r="C105">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="D105">
-        <f>5.67*10^-8*(B105+$E$1+273.14)^4</f>
+        <f t="shared" ref="D105:D136" si="6">5.67*10^-8*(B105+$E$1+273.14)^4</f>
         <v>384.85064865020979</v>
       </c>
       <c r="E105">
-        <f>5.67*10^-8*(C105+$E$2+273.14)^4</f>
-        <v>315.63697918226694</v>
+        <f t="shared" ref="E105:E136" si="7">5.67*10^-8*(C105+$E$2+273.14)^4</f>
+        <v>315.59075994061396</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -6825,11 +6830,11 @@
         <v>0.02</v>
       </c>
       <c r="D106">
-        <f>5.67*10^-8*(B106+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.40833870836519</v>
       </c>
       <c r="E106">
-        <f>5.67*10^-8*(C106+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>315.68320350044701</v>
       </c>
     </row>
@@ -6838,18 +6843,18 @@
         <v>1978</v>
       </c>
       <c r="B107">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C107">
-        <v>-0.28999999999999998</v>
+        <v>-0.3</v>
       </c>
       <c r="D107">
-        <f>5.67*10^-8*(B107+$E$1+273.14)^4</f>
-        <v>385.81693519898806</v>
+        <f t="shared" si="6"/>
+        <v>385.7632049269555</v>
       </c>
       <c r="E107">
-        <f>5.67*10^-8*(C107+$E$2+273.14)^4</f>
-        <v>314.25260855165118</v>
+        <f t="shared" si="7"/>
+        <v>314.20654143303597</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -6860,15 +6865,15 @@
         <v>0.16</v>
       </c>
       <c r="C108">
-        <v>-0.75</v>
+        <v>-0.77</v>
       </c>
       <c r="D108">
-        <f>5.67*10^-8*(B108+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.30076026079456</v>
       </c>
       <c r="E108">
-        <f>5.67*10^-8*(C108+$E$2+273.14)^4</f>
-        <v>312.13875774794229</v>
+        <f t="shared" si="7"/>
+        <v>312.04709377153983</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -6882,11 +6887,11 @@
         <v>0.15</v>
       </c>
       <c r="D109">
-        <f>5.67*10^-8*(B109+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.8388772055817</v>
       </c>
       <c r="E109">
-        <f>5.67*10^-8*(C109+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>316.28458176990767</v>
       </c>
     </row>
@@ -6901,11 +6906,11 @@
         <v>0.96</v>
       </c>
       <c r="D110">
-        <f>5.67*10^-8*(B110+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.21589343483623</v>
       </c>
       <c r="E110">
-        <f>5.67*10^-8*(C110+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>320.05100925822074</v>
       </c>
     </row>
@@ -6920,11 +6925,11 @@
         <v>-0.47</v>
       </c>
       <c r="D111">
-        <f>5.67*10^-8*(B111+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.13943470928126</v>
       </c>
       <c r="E111">
-        <f>5.67*10^-8*(C111+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>313.42417506033024</v>
       </c>
     </row>
@@ -6939,11 +6944,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D112">
-        <f>5.67*10^-8*(B112+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.10814640427151</v>
       </c>
       <c r="E112">
-        <f>5.67*10^-8*(C112+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>315.91440125226575</v>
       </c>
     </row>
@@ -6955,15 +6960,15 @@
         <v>0.16</v>
       </c>
       <c r="C113">
-        <v>0.55000000000000004</v>
+        <v>0.54</v>
       </c>
       <c r="D113">
-        <f>5.67*10^-8*(B113+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.30076026079456</v>
       </c>
       <c r="E113">
-        <f>5.67*10^-8*(C113+$E$2+273.14)^4</f>
-        <v>318.14036663080833</v>
+        <f t="shared" si="7"/>
+        <v>318.09387272443468</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -6977,11 +6982,11 @@
         <v>0.48</v>
       </c>
       <c r="D114">
-        <f>5.67*10^-8*(B114+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.0319124169402</v>
       </c>
       <c r="E114">
-        <f>5.67*10^-8*(C114+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>317.81501629433546</v>
       </c>
     </row>
@@ -6996,11 +7001,11 @@
         <v>-0.15</v>
       </c>
       <c r="D115">
-        <f>5.67*10^-8*(B115+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.35454667632962</v>
       </c>
       <c r="E115">
-        <f>5.67*10^-8*(C115+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>314.89808024635863</v>
       </c>
     </row>
@@ -7012,15 +7017,15 @@
         <v>0.31</v>
       </c>
       <c r="C116">
-        <v>-0.51</v>
+        <v>-0.52</v>
       </c>
       <c r="D116">
-        <f>5.67*10^-8*(B116+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.10814640427151</v>
       </c>
       <c r="E116">
-        <f>5.67*10^-8*(C116+$E$2+273.14)^4</f>
-        <v>313.24030138797718</v>
+        <f t="shared" si="7"/>
+        <v>313.19434561385918</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -7028,17 +7033,17 @@
         <v>1988</v>
       </c>
       <c r="B117">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="C117">
         <v>0.37</v>
       </c>
       <c r="D117">
-        <f>5.67*10^-8*(B117+$E$1+273.14)^4</f>
-        <v>387.48535941635276</v>
+        <f t="shared" si="6"/>
+        <v>387.5392694852323</v>
       </c>
       <c r="E117">
-        <f>5.67*10^-8*(C117+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>317.30425573794872</v>
       </c>
     </row>
@@ -7053,11 +7058,11 @@
         <v>0.12</v>
       </c>
       <c r="D118">
-        <f>5.67*10^-8*(B118+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.89271980371592</v>
       </c>
       <c r="E118">
-        <f>5.67*10^-8*(C118+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>316.14572597302583</v>
       </c>
     </row>
@@ -7072,11 +7077,11 @@
         <v>0.65</v>
       </c>
       <c r="D119">
-        <f>5.67*10^-8*(B119+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.80890421403086</v>
       </c>
       <c r="E119">
-        <f>5.67*10^-8*(C119+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>318.60558607004424</v>
       </c>
     </row>
@@ -7091,11 +7096,11 @@
         <v>0.67</v>
       </c>
       <c r="D120">
-        <f>5.67*10^-8*(B120+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.64710649869789</v>
       </c>
       <c r="E120">
-        <f>5.67*10^-8*(C120+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>318.6986911500984</v>
       </c>
     </row>
@@ -7110,11 +7115,11 @@
         <v>-0.28000000000000003</v>
       </c>
       <c r="D121">
-        <f>5.67*10^-8*(B121+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.62356300933067</v>
       </c>
       <c r="E121">
-        <f>5.67*10^-8*(C121+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>314.29868073564893</v>
       </c>
     </row>
@@ -7129,11 +7134,11 @@
         <v>0.46</v>
       </c>
       <c r="D122">
-        <f>5.67*10^-8*(B122+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>386.67738312973268</v>
       </c>
       <c r="E122">
-        <f>5.67*10^-8*(C122+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>317.72210490703856</v>
       </c>
     </row>
@@ -7148,11 +7153,11 @@
         <v>0.35</v>
       </c>
       <c r="D123">
-        <f>5.67*10^-8*(B123+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.16201710837066</v>
       </c>
       <c r="E123">
-        <f>5.67*10^-8*(C123+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>317.21145636568383</v>
       </c>
     </row>
@@ -7167,11 +7172,11 @@
         <v>1.26</v>
       </c>
       <c r="D124">
-        <f>5.67*10^-8*(B124+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.80890421403086</v>
       </c>
       <c r="E124">
-        <f>5.67*10^-8*(C124+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>321.45448316792823</v>
       </c>
     </row>
@@ -7186,11 +7191,11 @@
         <v>0.86</v>
       </c>
       <c r="D125">
-        <f>5.67*10^-8*(B125+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.26977538405936</v>
       </c>
       <c r="E125">
-        <f>5.67*10^-8*(C125+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>319.58420749919998</v>
       </c>
     </row>
@@ -7202,15 +7207,15 @@
         <v>0.46</v>
       </c>
       <c r="C126">
-        <v>0.62</v>
+        <v>0.63</v>
       </c>
       <c r="D126">
-        <f>5.67*10^-8*(B126+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.91679749224176</v>
       </c>
       <c r="E126">
-        <f>5.67*10^-8*(C126+$E$2+273.14)^4</f>
-        <v>318.46596670161199</v>
+        <f t="shared" si="7"/>
+        <v>318.5125013913663</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -7224,11 +7229,11 @@
         <v>0.95</v>
       </c>
       <c r="D127">
-        <f>5.67*10^-8*(B127+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>388.72671484522147</v>
       </c>
       <c r="E127">
-        <f>5.67*10^-8*(C127+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>320.0043060849211</v>
       </c>
     </row>
@@ -7240,15 +7245,15 @@
         <v>0.37</v>
       </c>
       <c r="C128">
-        <v>0.44</v>
+        <v>0.43</v>
       </c>
       <c r="D128">
-        <f>5.67*10^-8*(B128+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.43145497218694</v>
       </c>
       <c r="E128">
-        <f>5.67*10^-8*(C128+$E$2+273.14)^4</f>
-        <v>317.62921389281217</v>
+        <f t="shared" si="7"/>
+        <v>317.5827760246695</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -7262,11 +7267,11 @@
         <v>0.92</v>
       </c>
       <c r="D129">
-        <f>5.67*10^-8*(B129+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>387.59318517921673</v>
       </c>
       <c r="E129">
-        <f>5.67*10^-8*(C129+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>319.86422723269442</v>
       </c>
     </row>
@@ -7281,11 +7286,11 @@
         <v>1.07</v>
       </c>
       <c r="D130">
-        <f>5.67*10^-8*(B130+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>388.3485957501664</v>
       </c>
       <c r="E130">
-        <f>5.67*10^-8*(C130+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>320.56508163200465</v>
       </c>
     </row>
@@ -7297,15 +7302,15 @@
         <v>0.63</v>
       </c>
       <c r="C131">
-        <v>1.28</v>
+        <v>1.27</v>
       </c>
       <c r="D131">
-        <f>5.67*10^-8*(B131+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>388.83479956995308</v>
       </c>
       <c r="E131">
-        <f>5.67*10^-8*(C131+$E$2+273.14)^4</f>
-        <v>321.54821192283077</v>
+        <f t="shared" si="7"/>
+        <v>321.50134498364474</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -7316,15 +7321,15 @@
         <v>0.62</v>
       </c>
       <c r="C132">
-        <v>1.35</v>
+        <v>1.36</v>
       </c>
       <c r="D132">
-        <f>5.67*10^-8*(B132+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>388.78075439053333</v>
       </c>
       <c r="E132">
-        <f>5.67*10^-8*(C132+$E$2+273.14)^4</f>
-        <v>321.87642398565549</v>
+        <f t="shared" si="7"/>
+        <v>321.92333192604372</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -7332,18 +7337,18 @@
         <v>2004</v>
       </c>
       <c r="B133">
-        <v>0.53</v>
+        <v>0.54</v>
       </c>
       <c r="C133">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
       <c r="D133">
-        <f>5.67*10^-8*(B133+$E$1+273.14)^4</f>
-        <v>388.29460126362119</v>
+        <f t="shared" si="6"/>
+        <v>388.3485957501664</v>
       </c>
       <c r="E133">
-        <f>5.67*10^-8*(C133+$E$2+273.14)^4</f>
-        <v>317.1186773501102</v>
+        <f t="shared" si="7"/>
+        <v>317.16506431349643</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -7351,17 +7356,17 @@
         <v>2005</v>
       </c>
       <c r="B134">
-        <v>0.67</v>
+        <v>0.68</v>
       </c>
       <c r="C134">
         <v>2.0699999999999998</v>
       </c>
       <c r="D134">
-        <f>5.67*10^-8*(B134+$E$1+273.14)^4</f>
-        <v>389.05103663654262</v>
+        <f t="shared" si="6"/>
+        <v>389.10510999237562</v>
       </c>
       <c r="E134">
-        <f>5.67*10^-8*(C134+$E$2+273.14)^4</f>
+        <f t="shared" si="7"/>
         <v>325.26692216598116</v>
       </c>
     </row>
@@ -7373,15 +7378,15 @@
         <v>0.64</v>
       </c>
       <c r="C135">
-        <v>2.0299999999999998</v>
+        <v>2.04</v>
       </c>
       <c r="D135">
-        <f>5.67*10^-8*(B135+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>388.8888503838723</v>
       </c>
       <c r="E135">
-        <f>5.67*10^-8*(C135+$E$2+273.14)^4</f>
-        <v>325.07786158483344</v>
+        <f t="shared" si="7"/>
+        <v>325.12511900135144</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -7392,15 +7397,15 @@
         <v>0.67</v>
       </c>
       <c r="C136">
-        <v>2.27</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="D136">
-        <f>5.67*10^-8*(B136+$E$1+273.14)^4</f>
+        <f t="shared" si="6"/>
         <v>389.05103663654262</v>
       </c>
       <c r="E136">
-        <f>5.67*10^-8*(C136+$E$2+273.14)^4</f>
-        <v>326.21346236396727</v>
+        <f t="shared" si="7"/>
+        <v>325.97663389858718</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -7414,11 +7419,11 @@
         <v>1.69</v>
       </c>
       <c r="D137">
-        <f>5.67*10^-8*(B137+$E$1+273.14)^4</f>
+        <f t="shared" ref="D137:D153" si="8">5.67*10^-8*(B137+$E$1+273.14)^4</f>
         <v>388.3485957501664</v>
       </c>
       <c r="E137">
-        <f>5.67*10^-8*(C137+$E$2+273.14)^4</f>
+        <f t="shared" ref="E137:E153" si="9">5.67*10^-8*(C137+$E$2+273.14)^4</f>
         <v>323.47417234698594</v>
       </c>
     </row>
@@ -7430,15 +7435,15 @@
         <v>0.66</v>
       </c>
       <c r="C138">
-        <v>1.67</v>
+        <v>1.68</v>
       </c>
       <c r="D138">
-        <f>5.67*10^-8*(B138+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>388.99696891677559</v>
       </c>
       <c r="E138">
-        <f>5.67*10^-8*(C138+$E$2+273.14)^4</f>
-        <v>323.38002283954052</v>
+        <f t="shared" si="9"/>
+        <v>323.42709502386759</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -7446,18 +7451,18 @@
         <v>2010</v>
       </c>
       <c r="B139">
-        <v>0.72</v>
+        <v>0.73</v>
       </c>
       <c r="C139">
-        <v>2.46</v>
+        <v>2.5</v>
       </c>
       <c r="D139">
-        <f>5.67*10^-8*(B139+$E$1+273.14)^4</f>
-        <v>389.32145978420073</v>
+        <f t="shared" si="8"/>
+        <v>389.37556132623837</v>
       </c>
       <c r="E139">
-        <f>5.67*10^-8*(C139+$E$2+273.14)^4</f>
-        <v>327.11458761176817</v>
+        <f t="shared" si="9"/>
+        <v>327.30453583213392</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -7468,15 +7473,15 @@
         <v>0.61</v>
       </c>
       <c r="C140">
-        <v>2.68</v>
+        <v>2.65</v>
       </c>
       <c r="D140">
-        <f>5.67*10^-8*(B140+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>388.72671484522147</v>
       </c>
       <c r="E140">
-        <f>5.67*10^-8*(C140+$E$2+273.14)^4</f>
-        <v>328.16032673200743</v>
+        <f t="shared" si="9"/>
+        <v>328.0175785086895</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -7487,15 +7492,15 @@
         <v>0.64</v>
       </c>
       <c r="C141">
-        <v>2.74</v>
+        <v>2.65</v>
       </c>
       <c r="D141">
-        <f>5.67*10^-8*(B141+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>388.8888503838723</v>
       </c>
       <c r="E141">
-        <f>5.67*10^-8*(C141+$E$2+273.14)^4</f>
-        <v>328.44596294771134</v>
+        <f t="shared" si="9"/>
+        <v>328.0175785086895</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -7509,11 +7514,11 @@
         <v>1.64</v>
       </c>
       <c r="D142">
-        <f>5.67*10^-8*(B142+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>389.10510999237562</v>
       </c>
       <c r="E142">
-        <f>5.67*10^-8*(C142+$E$2+273.14)^4</f>
+        <f t="shared" si="9"/>
         <v>323.23883711556692</v>
       </c>
     </row>
@@ -7522,18 +7527,18 @@
         <v>2014</v>
       </c>
       <c r="B143">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
       <c r="C143">
-        <v>2.2000000000000002</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="D143">
-        <f>5.67*10^-8*(B143+$E$1+273.14)^4</f>
-        <v>389.42966850669217</v>
+        <f t="shared" si="8"/>
+        <v>389.48378132595394</v>
       </c>
       <c r="E143">
-        <f>5.67*10^-8*(C143+$E$2+273.14)^4</f>
-        <v>325.88193862809806</v>
+        <f t="shared" si="9"/>
+        <v>325.97663389858718</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -7544,15 +7549,15 @@
         <v>0.89</v>
       </c>
       <c r="C144">
-        <v>2.1800000000000002</v>
+        <v>2.21</v>
       </c>
       <c r="D144">
-        <f>5.67*10^-8*(B144+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>390.24195308984537</v>
       </c>
       <c r="E144">
-        <f>5.67*10^-8*(C144+$E$2+273.14)^4</f>
-        <v>325.78726399063476</v>
+        <f t="shared" si="9"/>
+        <v>325.92928368402693</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -7563,15 +7568,15 @@
         <v>1.02</v>
       </c>
       <c r="C145">
-        <v>3.66</v>
+        <v>3.65</v>
       </c>
       <c r="D145">
-        <f>5.67*10^-8*(B145+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>390.94696034716645</v>
       </c>
       <c r="E145">
-        <f>5.67*10^-8*(C145+$E$2+273.14)^4</f>
-        <v>332.84911152955391</v>
+        <f t="shared" si="9"/>
+        <v>332.80101455345243</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -7585,11 +7590,11 @@
         <v>2.7</v>
       </c>
       <c r="D146">
-        <f>5.67*10^-8*(B146+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>390.4045623706611</v>
       </c>
       <c r="E146">
-        <f>5.67*10^-8*(C146+$E$2+273.14)^4</f>
+        <f t="shared" si="9"/>
         <v>328.25551809487763</v>
       </c>
     </row>
@@ -7601,15 +7606,15 @@
         <v>0.85</v>
       </c>
       <c r="C147">
-        <v>2.4</v>
+        <v>2.42</v>
       </c>
       <c r="D147">
-        <f>5.67*10^-8*(B147+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>390.02521973919369</v>
       </c>
       <c r="E147">
-        <f>5.67*10^-8*(C147+$E$2+273.14)^4</f>
-        <v>326.82982031380078</v>
+        <f t="shared" si="9"/>
+        <v>326.92472207944598</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -7617,18 +7622,18 @@
         <v>2019</v>
       </c>
       <c r="B148">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="C148">
-        <v>2.84</v>
+        <v>2.91</v>
       </c>
       <c r="D148">
-        <f>5.67*10^-8*(B148+$E$1+273.14)^4</f>
-        <v>390.67569076114364</v>
+        <f t="shared" si="8"/>
+        <v>390.72993338113662</v>
       </c>
       <c r="E148">
-        <f>5.67*10^-8*(C148+$E$2+273.14)^4</f>
-        <v>328.92243762799313</v>
+        <f t="shared" si="9"/>
+        <v>329.25627822655298</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -7636,18 +7641,18 @@
         <v>2020</v>
       </c>
       <c r="B149">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="C149">
-        <v>3.15</v>
+        <v>3.1</v>
       </c>
       <c r="D149">
-        <f>5.67*10^-8*(B149+$E$1+273.14)^4</f>
-        <v>390.94696034716645</v>
+        <f t="shared" si="8"/>
+        <v>390.89269513196621</v>
       </c>
       <c r="E149">
-        <f>5.67*10^-8*(C149+$E$2+273.14)^4</f>
-        <v>330.4028041367705</v>
+        <f t="shared" si="9"/>
+        <v>330.16369803388989</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -7658,15 +7663,72 @@
         <v>0.85</v>
       </c>
       <c r="C150">
-        <v>2.42</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="D150">
-        <f>5.67*10^-8*(B150+$E$1+273.14)^4</f>
+        <f t="shared" si="8"/>
         <v>390.02521973919369</v>
       </c>
       <c r="E150">
-        <f>5.67*10^-8*(C150+$E$2+273.14)^4</f>
-        <v>326.92472207944598</v>
+        <f t="shared" si="9"/>
+        <v>327.06711347762115</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>2022</v>
+      </c>
+      <c r="B151">
+        <v>0.9</v>
+      </c>
+      <c r="C151">
+        <v>2.54</v>
+      </c>
+      <c r="D151">
+        <f t="shared" si="8"/>
+        <v>390.29615053824244</v>
+      </c>
+      <c r="E151">
+        <f t="shared" si="9"/>
+        <v>327.49456676454707</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>2023</v>
+      </c>
+      <c r="B152">
+        <v>1.17</v>
+      </c>
+      <c r="C152">
+        <v>2.79</v>
+      </c>
+      <c r="D152">
+        <f t="shared" si="8"/>
+        <v>391.76161676863984</v>
+      </c>
+      <c r="E152">
+        <f t="shared" si="9"/>
+        <v>328.68413553302315</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>2024</v>
+      </c>
+      <c r="B153">
+        <v>1.29</v>
+      </c>
+      <c r="C153">
+        <v>3.15</v>
+      </c>
+      <c r="D153">
+        <f t="shared" si="8"/>
+        <v>392.4142580601096</v>
+      </c>
+      <c r="E153">
+        <f t="shared" si="9"/>
+        <v>330.4028041367705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding both 2021 file (original) and 2024 file
</commit_message>
<xml_diff>
--- a/GISTEMP_Arctic_Global_SurfaceTemperature_1880-2021_withLongwaveRadiation.xlsx
+++ b/GISTEMP_Arctic_Global_SurfaceTemperature_1880-2021_withLongwaveRadiation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeka1927/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jen/Documents/jenkay/jek_proposals/2016_NSF_CAREER/Curriculum/v2_data_through2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC500A-6432-EE4E-8F08-BD9B39390170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0A6459-7EC8-C54D-9C87-D75801B13E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="500" windowWidth="30700" windowHeight="25260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="460" windowWidth="23240" windowHeight="24880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LWgraph" sheetId="2" r:id="rId1"/>
@@ -22,12 +22,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -49,6 +44,9 @@
     <t xml:space="preserve"> Hansen et al. 2010; anomaly calculated with respect to 1951-1980 base period </t>
   </si>
   <si>
+    <t xml:space="preserve">Data were downloaded April 2019 from http://www.esrl.noaa.gov/psd/data/gridded/data.gistemp.html </t>
+  </si>
+  <si>
     <t>Global mean temperature (1951-1980) in deg C</t>
   </si>
   <si>
@@ -56,6 +54,9 @@
   </si>
   <si>
     <t>Global blackbody longwave radiation emitted (Wm-2)</t>
+  </si>
+  <si>
+    <t>Data munged by Jennifer.E.Kay@colorado.edu using GISTEMP_timeseries_through2021.ncl</t>
   </si>
   <si>
     <t xml:space="preserve"> last update March 2022 </t>
@@ -68,12 +69,6 @@
   </si>
   <si>
     <t>Arctic mean temperature (estimate) in deg C</t>
-  </si>
-  <si>
-    <t>Data munged by Jennifer.E.Kay@colorado.edu using GISTEMP_timeseries_through2024.ncl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data were downloaded May 2024 from http://www.esrl.noaa.gov/psd/data/gridded/data.gistemp.html </t>
   </si>
 </sst>
 </file>
@@ -767,10 +762,10 @@
                   <c:v>388.78075439053333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>388.3485957501664</c:v>
+                  <c:v>388.29460126362119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>389.10510999237562</c:v>
+                  <c:v>389.05103663654262</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>388.8888503838723</c:v>
@@ -785,7 +780,7 @@
                   <c:v>388.99696891677559</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>389.37556132623837</c:v>
+                  <c:v>389.32145978420073</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>388.72671484522147</c:v>
@@ -797,7 +792,7 @@
                   <c:v>389.10510999237562</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>389.48378132595394</c:v>
+                  <c:v>389.42966850669217</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>390.24195308984537</c:v>
@@ -812,10 +807,10 @@
                   <c:v>390.02521973919369</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>390.72993338113662</c:v>
+                  <c:v>390.67569076114364</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>390.89269513196621</c:v>
+                  <c:v>390.94696034716645</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>390.02521973919369</c:v>
@@ -944,64 +939,64 @@
                   <c:v>320.56508163200465</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>321.50134498364474</c:v>
+                  <c:v>321.54821192283077</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>321.92333192604372</c:v>
+                  <c:v>321.87642398565549</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>317.16506431349643</c:v>
+                  <c:v>317.1186773501102</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>325.26692216598116</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>325.12511900135144</c:v>
+                  <c:v>325.07786158483344</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>325.97663389858718</c:v>
+                  <c:v>326.21346236396727</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>323.47417234698594</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>323.42709502386759</c:v>
+                  <c:v>323.38002283954052</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>327.30453583213392</c:v>
+                  <c:v>327.11458761176817</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>328.0175785086895</c:v>
+                  <c:v>328.16032673200743</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>328.0175785086895</c:v>
+                  <c:v>328.44596294771134</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>323.23883711556692</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>325.97663389858718</c:v>
+                  <c:v>325.88193862809806</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>325.92928368402693</c:v>
+                  <c:v>325.78726399063476</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>332.80101455345243</c:v>
+                  <c:v>332.84911152955391</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>328.25551809487763</c:v>
                 </c:pt>
                 <c:pt idx="18">
+                  <c:v>326.82982031380078</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>328.92243762799313</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>330.4028041367705</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>326.92472207944598</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>329.25627822655298</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>330.16369803388989</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>327.06711347762115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1252,7 +1247,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1260,6 +1254,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1787,40 +1782,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="142"/>
                 <c:pt idx="0">
-                  <c:v>384.36818659357857</c:v>
+                  <c:v>384.47536115961219</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>384.74339563096243</c:v>
+                  <c:v>384.85064865020979</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>384.68977752870001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>384.31460771382257</c:v>
+                  <c:v>384.36818659357857</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>383.72560965972832</c:v>
+                  <c:v>383.77912694277103</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>383.51159649724525</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>383.61859188532998</c:v>
+                  <c:v>383.67209797404479</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>383.40462349235258</c:v>
+                  <c:v>383.4581071970951</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>384.36818659357857</c:v>
+                  <c:v>384.42177107537833</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>384.79701933800214</c:v>
+                  <c:v>384.85064865020979</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>383.4581071970951</c:v>
+                  <c:v>383.51159649724525</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>384.2074667588796</c:v>
+                  <c:v>384.26103443571941</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>383.83264982356309</c:v>
@@ -1829,91 +1824,91 @@
                   <c:v>383.72560965972832</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>383.72560965972832</c:v>
+                  <c:v>383.77912694277103</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>384.15390468291196</c:v>
+                  <c:v>384.2074667588796</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>384.63616503082426</c:v>
+                  <c:v>384.68977752870001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>384.74339563096243</c:v>
+                  <c:v>384.79701933800214</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>383.83264982356309</c:v>
+                  <c:v>383.93971237995703</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>384.36818659357857</c:v>
+                  <c:v>384.47536115961219</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>384.90428356797594</c:v>
+                  <c:v>384.95792409169127</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>384.52895684667084</c:v>
+                  <c:v>384.58255813694461</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>383.83264982356309</c:v>
+                  <c:v>383.8861783024949</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>383.35114538262775</c:v>
+                  <c:v>383.40462349235258</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>382.97695524226617</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>384.0467973320321</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>384.26103443571941</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>383.29767286753008</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>383.19074461965545</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>382.87009410650859</c:v>
                 </c:pt>
-                <c:pt idx="25">
-                  <c:v>383.9932520563392</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>384.2074667588796</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>383.24420594666913</c:v>
-                </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="30">
                   <c:v>383.13728888609842</c:v>
                 </c:pt>
-                <c:pt idx="29">
-                  <c:v>382.76325533521504</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>383.0303941977939</c:v>
-                </c:pt>
                 <c:pt idx="31">
-                  <c:v>383.0303941977939</c:v>
+                  <c:v>383.08383874560803</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>383.4581071970951</c:v>
+                  <c:v>383.51159649724525</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>383.4581071970951</c:v>
+                  <c:v>383.56509139319331</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>384.47536115961219</c:v>
+                  <c:v>384.58255813694461</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>384.63616503082426</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>383.40462349235258</c:v>
+                  <c:v>383.51159649724525</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>382.87009410650859</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>383.72560965972832</c:v>
+                  <c:v>383.77912694277103</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>383.8861783024949</c:v>
                 </c:pt>
                 <c:pt idx="40">
+                  <c:v>383.93971237995703</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>384.42177107537833</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>383.8861783024949</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>384.36818659357857</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>383.83264982356309</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>383.9932520563392</c:v>
@@ -1922,13 +1917,13 @@
                   <c:v>383.9932520563392</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>384.2074667588796</c:v>
+                  <c:v>384.26103443571941</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>384.90428356797594</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>384.26103443571941</c:v>
+                  <c:v>384.31460771382257</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>384.36818659357857</c:v>
@@ -1946,37 +1941,37 @@
                   <c:v>384.63616503082426</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>383.8861783024949</c:v>
+                  <c:v>383.93971237995703</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>384.79701933800214</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>384.36818659357857</c:v>
+                  <c:v>384.42177107537833</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>384.68977752870001</c:v>
+                  <c:v>384.74339563096243</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>385.33356475708479</c:v>
+                  <c:v>385.38725014245563</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>385.44094113729142</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>385.33356475708479</c:v>
+                  <c:v>385.38725014245563</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>386.1932042776611</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>386.46213635729197</c:v>
+                  <c:v>386.51593962350103</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>385.81693519898806</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>385.92441258121801</c:v>
+                  <c:v>385.97815969219738</c:v>
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>386.51593962350103</c:v>
@@ -1997,10 +1992,10 @@
                   <c:v>384.85064865020979</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>384.47536115961219</c:v>
+                  <c:v>384.52895684667084</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>385.06522195853137</c:v>
+                  <c:v>385.11887930243745</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>385.49463774198318</c:v>
@@ -2024,7 +2019,7 @@
                   <c:v>385.7632049269555</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>385.54833995692138</c:v>
+                  <c:v>385.60204778249698</c:v>
                 </c:pt>
                 <c:pt idx="80">
                   <c:v>385.27988498078827</c:v>
@@ -2060,7 +2055,7 @@
                   <c:v>385.54833995692138</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>385.01157022174618</c:v>
+                  <c:v>384.95792409169127</c:v>
                 </c:pt>
                 <c:pt idx="92">
                   <c:v>385.44094113729142</c:v>
@@ -2081,7 +2076,7 @@
                   <c:v>386.40833870836519</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>385.7632049269555</c:v>
+                  <c:v>385.81693519898806</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>386.30076026079456</c:v>
@@ -2111,7 +2106,7 @@
                   <c:v>387.10814640427151</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>387.5392694852323</c:v>
+                  <c:v>387.48535941635276</c:v>
                 </c:pt>
                 <c:pt idx="109">
                   <c:v>386.89271980371592</c:v>
@@ -2159,10 +2154,10 @@
                   <c:v>388.78075439053333</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>388.3485957501664</c:v>
+                  <c:v>388.29460126362119</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>389.10510999237562</c:v>
+                  <c:v>389.05103663654262</c:v>
                 </c:pt>
                 <c:pt idx="126">
                   <c:v>388.8888503838723</c:v>
@@ -2177,7 +2172,7 @@
                   <c:v>388.99696891677559</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>389.37556132623837</c:v>
+                  <c:v>389.32145978420073</c:v>
                 </c:pt>
                 <c:pt idx="131">
                   <c:v>388.72671484522147</c:v>
@@ -2189,7 +2184,7 @@
                   <c:v>389.10510999237562</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>389.48378132595394</c:v>
+                  <c:v>389.42966850669217</c:v>
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>390.24195308984537</c:v>
@@ -2204,10 +2199,10 @@
                   <c:v>390.02521973919369</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>390.72993338113662</c:v>
+                  <c:v>390.67569076114364</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>390.89269513196621</c:v>
+                  <c:v>390.94696034716645</c:v>
                 </c:pt>
                 <c:pt idx="141">
                   <c:v>390.02521973919369</c:v>
@@ -2690,25 +2685,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="142"/>
                 <c:pt idx="0">
-                  <c:v>310.94870005051018</c:v>
+                  <c:v>311.04012193891896</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>310.44623985076419</c:v>
+                  <c:v>310.53755092477502</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>307.48957589571449</c:v>
+                  <c:v>307.44425436720354</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>314.9903715939945</c:v>
+                  <c:v>314.85194217859879</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>310.81160500710308</c:v>
+                  <c:v>310.6745553018572</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>306.90078671588617</c:v>
+                  <c:v>306.76503245802877</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>305.40996554885356</c:v>
+                  <c:v>305.36487410804472</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>306.17728436537561</c:v>
@@ -2717,7 +2712,7 @@
                   <c:v>309.12449083844746</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>311.58907668477633</c:v>
+                  <c:v>311.63485568992365</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>310.49189287027872</c:v>
@@ -2726,64 +2721,64 @@
                   <c:v>309.67090851259422</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>309.352076914723</c:v>
+                  <c:v>309.39760920569358</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>312.59738058829214</c:v>
+                  <c:v>312.64327065234374</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>309.5797886342898</c:v>
+                  <c:v>309.76204850418208</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>311.72642883331054</c:v>
+                  <c:v>311.90963566282767</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>310.72023349998278</c:v>
+                  <c:v>310.90299666451727</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>312.68916576879064</c:v>
+                  <c:v>312.82688143621107</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>308.66969543087725</c:v>
+                  <c:v>308.76061433907716</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>309.03349157770413</c:v>
+                  <c:v>309.07898869631936</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>312.09292323576784</c:v>
+                  <c:v>312.13875774794229</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>312.09292323576784</c:v>
+                  <c:v>312.00126935488771</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>307.85232853569312</c:v>
+                  <c:v>308.62424350724052</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>313.51614224722954</c:v>
+                  <c:v>313.6541309743302</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>314.06837046577078</c:v>
+                  <c:v>314.52911764936545</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>314.89808024635863</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>314.29868073564893</c:v>
+                  <c:v>314.34475798539989</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>312.87279676594761</c:v>
+                  <c:v>312.91871714993346</c:v>
                 </c:pt>
                 <c:pt idx="28">
                   <c:v>314.25260855165118</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>312.00126935488771</c:v>
+                  <c:v>312.04709377153983</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>311.81802215662361</c:v>
+                  <c:v>312.68916576879064</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>313.79216524644022</c:v>
+                  <c:v>313.74614876122854</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>312.55149557626464</c:v>
@@ -2792,100 +2787,100 @@
                   <c:v>312.00126935488771</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>313.28626221931233</c:v>
+                  <c:v>313.33222810823565</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>312.04709377153983</c:v>
+                  <c:v>311.17729256814567</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>312.64327065234374</c:v>
+                  <c:v>313.05650863109679</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>310.44623985076419</c:v>
+                  <c:v>309.48868886630936</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>309.85320861201268</c:v>
+                  <c:v>310.08119690957619</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>312.18459730843387</c:v>
+                  <c:v>311.54330272349921</c:v>
                 </c:pt>
                 <c:pt idx="40">
+                  <c:v>315.22118871776757</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>314.9903715939945</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>313.97628180769811</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>316.70142361426849</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>316.8868188521655</c:v>
+                </c:pt>
+                <c:pt idx="45">
                   <c:v>315.03652487461358</c:v>
                 </c:pt>
-                <c:pt idx="41">
-                  <c:v>314.89808024635863</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>314.34475798539989</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>316.8868188521655</c:v>
-                </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="46">
+                  <c:v>317.62921389281217</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>315.86815154587384</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>319.44426659779566</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>316.9795469890347</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>319.11791655729439</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>318.93154312581487</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>318.60558607004424</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>316.05318084547457</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>320.28460181068391</c:v>
+                </c:pt>
+                <c:pt idx="55">
                   <c:v>317.67565685347773</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>315.26736736058308</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>317.7685580538672</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>315.91440125226575</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>319.16452267534032</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>316.8868188521655</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>319.02471963415906</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>319.02471963415906</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>318.5125013913663</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>316.1920061575405</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>320.42481870436319</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>317.48991556446401</c:v>
-                </c:pt>
                 <c:pt idx="56">
-                  <c:v>318.5125013913663</c:v>
+                  <c:v>318.3729126194097</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>322.2987800464457</c:v>
+                  <c:v>322.34573414176174</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>324.3696183540489</c:v>
+                  <c:v>324.18094910305086</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>318.41943711108399</c:v>
+                  <c:v>318.46596670161199</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>320.89254087405959</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>315.72943289552609</c:v>
+                  <c:v>315.59075994061396</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>320.05100925822074</c:v>
+                  <c:v>319.95760802314891</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>322.62756646079947</c:v>
+                  <c:v>322.5336018286975</c:v>
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>321.22025092832246</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>319.72419437414351</c:v>
+                  <c:v>319.63086468217966</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>315.91440125226575</c:v>
@@ -2897,43 +2892,43 @@
                   <c:v>315.22118871776757</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>316.51610973765031</c:v>
+                  <c:v>316.56243058048676</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>317.02591868825147</c:v>
+                  <c:v>317.1186773501102</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>315.82190691786786</c:v>
+                  <c:v>315.86815154587384</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>317.90794805768098</c:v>
+                  <c:v>317.86147962881603</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>320.89254087405959</c:v>
+                  <c:v>320.79895550313137</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>320.47156789819479</c:v>
+                  <c:v>320.51832220728426</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>314.89808024635863</c:v>
+                  <c:v>314.85194217859879</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>316.9795469890347</c:v>
+                  <c:v>316.93318037713016</c:v>
                 </c:pt>
                 <c:pt idx="77">
                   <c:v>315.96065603741522</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>315.08268322692891</c:v>
+                  <c:v>315.17501514813443</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>318.2333697337848</c:v>
+                  <c:v>318.18686563380078</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>317.35066305877109</c:v>
+                  <c:v>317.30425573794872</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>314.57522023345405</c:v>
+                  <c:v>314.62132788552441</c:v>
                 </c:pt>
                 <c:pt idx="82">
                   <c:v>317.07229547515254</c:v>
@@ -2942,7 +2937,7 @@
                   <c:v>313.56213342965839</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>312.32214628351784</c:v>
+                  <c:v>312.23044191761312</c:v>
                 </c:pt>
                 <c:pt idx="85">
                   <c:v>314.80580918104931</c:v>
@@ -2957,37 +2952,37 @@
                   <c:v>313.28626221931233</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>315.91440125226575</c:v>
+                  <c:v>315.86815154587384</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>314.39084030127572</c:v>
+                  <c:v>314.29868073564893</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>315.40593373183998</c:v>
+                  <c:v>315.3597398672477</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>314.85194217859879</c:v>
+                  <c:v>314.89808024635863</c:v>
                 </c:pt>
                 <c:pt idx="93">
+                  <c:v>315.31355107695254</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>315.03652487461358</c:v>
+                </c:pt>
+                <c:pt idx="95">
                   <c:v>315.22118871776757</c:v>
                 </c:pt>
-                <c:pt idx="94">
-                  <c:v>315.08268322692891</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>315.26736736058308</c:v>
-                </c:pt>
                 <c:pt idx="96">
-                  <c:v>315.59075994061396</c:v>
+                  <c:v>315.63697918226694</c:v>
                 </c:pt>
                 <c:pt idx="97">
                   <c:v>315.68320350044701</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>314.20654143303597</c:v>
+                  <c:v>314.25260855165118</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>312.04709377153983</c:v>
+                  <c:v>312.13875774794229</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>316.28458176990767</c:v>
@@ -3002,7 +2997,7 @@
                   <c:v>315.91440125226575</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>318.09387272443468</c:v>
+                  <c:v>318.14036663080833</c:v>
                 </c:pt>
                 <c:pt idx="105">
                   <c:v>317.81501629433546</c:v>
@@ -3011,7 +3006,7 @@
                   <c:v>314.89808024635863</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>313.19434561385918</c:v>
+                  <c:v>313.24030138797718</c:v>
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>317.30425573794872</c:v>
@@ -3041,13 +3036,13 @@
                   <c:v>319.58420749919998</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>318.5125013913663</c:v>
+                  <c:v>318.46596670161199</c:v>
                 </c:pt>
                 <c:pt idx="118">
                   <c:v>320.0043060849211</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>317.5827760246695</c:v>
+                  <c:v>317.62921389281217</c:v>
                 </c:pt>
                 <c:pt idx="120">
                   <c:v>319.86422723269442</c:v>
@@ -3056,64 +3051,64 @@
                   <c:v>320.56508163200465</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>321.50134498364474</c:v>
+                  <c:v>321.54821192283077</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>321.92333192604372</c:v>
+                  <c:v>321.87642398565549</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>317.16506431349643</c:v>
+                  <c:v>317.1186773501102</c:v>
                 </c:pt>
                 <c:pt idx="125">
                   <c:v>325.26692216598116</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>325.12511900135144</c:v>
+                  <c:v>325.07786158483344</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>325.97663389858718</c:v>
+                  <c:v>326.21346236396727</c:v>
                 </c:pt>
                 <c:pt idx="128">
                   <c:v>323.47417234698594</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>323.42709502386759</c:v>
+                  <c:v>323.38002283954052</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>327.30453583213392</c:v>
+                  <c:v>327.11458761176817</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>328.0175785086895</c:v>
+                  <c:v>328.16032673200743</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>328.0175785086895</c:v>
+                  <c:v>328.44596294771134</c:v>
                 </c:pt>
                 <c:pt idx="133">
                   <c:v>323.23883711556692</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>325.97663389858718</c:v>
+                  <c:v>325.88193862809806</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>325.92928368402693</c:v>
+                  <c:v>325.78726399063476</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>332.80101455345243</c:v>
+                  <c:v>332.84911152955391</c:v>
                 </c:pt>
                 <c:pt idx="137">
                   <c:v>328.25551809487763</c:v>
                 </c:pt>
                 <c:pt idx="138">
+                  <c:v>326.82982031380078</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>328.92243762799313</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>330.4028041367705</c:v>
+                </c:pt>
+                <c:pt idx="141">
                   <c:v>326.92472207944598</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>329.25627822655298</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>330.16369803388989</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>327.06711347762115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3364,7 +3359,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3372,6 +3366,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -4517,7 +4512,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="208" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="168" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4528,7 +4523,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1904E8C6-5EA8-F24D-9F1F-2EE48A32A0CE}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="208" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="168" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4539,7 +4534,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8676298" cy="6288942"/>
+    <xdr:ext cx="8670774" cy="6281964"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4572,7 +4567,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8670774" cy="6281964"/>
+    <xdr:ext cx="8676913" cy="6281812"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4602,9 +4597,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4642,7 +4637,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -4748,7 +4743,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4890,7 +4885,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4898,10 +4893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E153"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4914,7 +4909,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E1">
         <v>14</v>
@@ -4925,7 +4920,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -4946,15 +4941,15 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4964,16 +4959,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
         <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -4981,18 +4976,18 @@
         <v>1880</v>
       </c>
       <c r="B9">
-        <v>-0.2</v>
+        <v>-0.18</v>
       </c>
       <c r="C9">
-        <v>-1.01</v>
+        <v>-0.99</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D40" si="0">5.67*10^-8*(B9+$E$1+273.14)^4</f>
-        <v>384.36818659357857</v>
+        <f>5.67*10^-8*(B9+$E$1+273.14)^4</f>
+        <v>384.47536115961219</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E40" si="1">5.67*10^-8*(C9+$E$2+273.14)^4</f>
-        <v>310.94870005051018</v>
+        <f>5.67*10^-8*(C9+$E$2+273.14)^4</f>
+        <v>311.04012193891896</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -5000,18 +4995,18 @@
         <v>1881</v>
       </c>
       <c r="B10">
-        <v>-0.13</v>
+        <v>-0.11</v>
       </c>
       <c r="C10">
-        <v>-1.1200000000000001</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
-        <v>384.74339563096243</v>
+        <f>5.67*10^-8*(B10+$E$1+273.14)^4</f>
+        <v>384.85064865020979</v>
       </c>
       <c r="E10">
-        <f t="shared" si="1"/>
-        <v>310.44623985076419</v>
+        <f>5.67*10^-8*(C10+$E$2+273.14)^4</f>
+        <v>310.53755092477502</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -5022,15 +5017,15 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C11">
-        <v>-1.77</v>
+        <v>-1.78</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f>5.67*10^-8*(B11+$E$1+273.14)^4</f>
         <v>384.68977752870001</v>
       </c>
       <c r="E11">
-        <f t="shared" si="1"/>
-        <v>307.48957589571449</v>
+        <f>5.67*10^-8*(C11+$E$2+273.14)^4</f>
+        <v>307.44425436720354</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5038,18 +5033,18 @@
         <v>1883</v>
       </c>
       <c r="B12">
-        <v>-0.21</v>
+        <v>-0.2</v>
       </c>
       <c r="C12">
-        <v>-0.13</v>
+        <v>-0.16</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>384.31460771382257</v>
+        <f>5.67*10^-8*(B12+$E$1+273.14)^4</f>
+        <v>384.36818659357857</v>
       </c>
       <c r="E12">
-        <f t="shared" si="1"/>
-        <v>314.9903715939945</v>
+        <f>5.67*10^-8*(C12+$E$2+273.14)^4</f>
+        <v>314.85194217859879</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -5057,18 +5052,18 @@
         <v>1884</v>
       </c>
       <c r="B13">
-        <v>-0.32</v>
+        <v>-0.31</v>
       </c>
       <c r="C13">
-        <v>-1.04</v>
+        <v>-1.07</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>383.72560965972832</v>
+        <f>5.67*10^-8*(B13+$E$1+273.14)^4</f>
+        <v>383.77912694277103</v>
       </c>
       <c r="E13">
-        <f t="shared" si="1"/>
-        <v>310.81160500710308</v>
+        <f>5.67*10^-8*(C13+$E$2+273.14)^4</f>
+        <v>310.6745553018572</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -5079,15 +5074,15 @@
         <v>-0.36</v>
       </c>
       <c r="C14">
-        <v>-1.9</v>
+        <v>-1.93</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f>5.67*10^-8*(B14+$E$1+273.14)^4</f>
         <v>383.51159649724525</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
-        <v>306.90078671588617</v>
+        <f>5.67*10^-8*(C14+$E$2+273.14)^4</f>
+        <v>306.76503245802877</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5095,18 +5090,18 @@
         <v>1886</v>
       </c>
       <c r="B15">
-        <v>-0.34</v>
+        <v>-0.33</v>
       </c>
       <c r="C15">
-        <v>-2.23</v>
+        <v>-2.2400000000000002</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>383.61859188532998</v>
+        <f>5.67*10^-8*(B15+$E$1+273.14)^4</f>
+        <v>383.67209797404479</v>
       </c>
       <c r="E15">
-        <f t="shared" si="1"/>
-        <v>305.40996554885356</v>
+        <f>5.67*10^-8*(C15+$E$2+273.14)^4</f>
+        <v>305.36487410804472</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -5114,17 +5109,17 @@
         <v>1887</v>
       </c>
       <c r="B16">
-        <v>-0.38</v>
+        <v>-0.37</v>
       </c>
       <c r="C16">
         <v>-2.06</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>383.40462349235258</v>
+        <f>5.67*10^-8*(B16+$E$1+273.14)^4</f>
+        <v>383.4581071970951</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f>5.67*10^-8*(C16+$E$2+273.14)^4</f>
         <v>306.17728436537561</v>
       </c>
     </row>
@@ -5133,17 +5128,17 @@
         <v>1888</v>
       </c>
       <c r="B17">
-        <v>-0.2</v>
+        <v>-0.19</v>
       </c>
       <c r="C17">
         <v>-1.41</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>384.36818659357857</v>
+        <f>5.67*10^-8*(B17+$E$1+273.14)^4</f>
+        <v>384.42177107537833</v>
       </c>
       <c r="E17">
-        <f t="shared" si="1"/>
+        <f>5.67*10^-8*(C17+$E$2+273.14)^4</f>
         <v>309.12449083844746</v>
       </c>
     </row>
@@ -5152,18 +5147,18 @@
         <v>1889</v>
       </c>
       <c r="B18">
-        <v>-0.12</v>
+        <v>-0.11</v>
       </c>
       <c r="C18">
-        <v>-0.87</v>
+        <v>-0.86</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>384.79701933800214</v>
+        <f>5.67*10^-8*(B18+$E$1+273.14)^4</f>
+        <v>384.85064865020979</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
-        <v>311.58907668477633</v>
+        <f>5.67*10^-8*(C18+$E$2+273.14)^4</f>
+        <v>311.63485568992365</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -5171,17 +5166,17 @@
         <v>1890</v>
       </c>
       <c r="B19">
-        <v>-0.37</v>
+        <v>-0.36</v>
       </c>
       <c r="C19">
         <v>-1.1100000000000001</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
-        <v>383.4581071970951</v>
+        <f>5.67*10^-8*(B19+$E$1+273.14)^4</f>
+        <v>383.51159649724525</v>
       </c>
       <c r="E19">
-        <f t="shared" si="1"/>
+        <f>5.67*10^-8*(C19+$E$2+273.14)^4</f>
         <v>310.49189287027872</v>
       </c>
     </row>
@@ -5190,17 +5185,17 @@
         <v>1891</v>
       </c>
       <c r="B20">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
       <c r="C20">
         <v>-1.29</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
-        <v>384.2074667588796</v>
+        <f>5.67*10^-8*(B20+$E$1+273.14)^4</f>
+        <v>384.26103443571941</v>
       </c>
       <c r="E20">
-        <f t="shared" si="1"/>
+        <f>5.67*10^-8*(C20+$E$2+273.14)^4</f>
         <v>309.67090851259422</v>
       </c>
     </row>
@@ -5212,15 +5207,15 @@
         <v>-0.3</v>
       </c>
       <c r="C21">
-        <v>-1.36</v>
+        <v>-1.35</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f>5.67*10^-8*(B21+$E$1+273.14)^4</f>
         <v>383.83264982356309</v>
       </c>
       <c r="E21">
-        <f t="shared" si="1"/>
-        <v>309.352076914723</v>
+        <f>5.67*10^-8*(C21+$E$2+273.14)^4</f>
+        <v>309.39760920569358</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -5231,15 +5226,15 @@
         <v>-0.32</v>
       </c>
       <c r="C22">
-        <v>-0.65</v>
+        <v>-0.64</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f>5.67*10^-8*(B22+$E$1+273.14)^4</f>
         <v>383.72560965972832</v>
       </c>
       <c r="E22">
-        <f t="shared" si="1"/>
-        <v>312.59738058829214</v>
+        <f>5.67*10^-8*(C22+$E$2+273.14)^4</f>
+        <v>312.64327065234374</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -5247,18 +5242,18 @@
         <v>1894</v>
       </c>
       <c r="B23">
-        <v>-0.32</v>
+        <v>-0.31</v>
       </c>
       <c r="C23">
-        <v>-1.31</v>
+        <v>-1.27</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
-        <v>383.72560965972832</v>
+        <f>5.67*10^-8*(B23+$E$1+273.14)^4</f>
+        <v>383.77912694277103</v>
       </c>
       <c r="E23">
-        <f t="shared" si="1"/>
-        <v>309.5797886342898</v>
+        <f>5.67*10^-8*(C23+$E$2+273.14)^4</f>
+        <v>309.76204850418208</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -5266,18 +5261,18 @@
         <v>1895</v>
       </c>
       <c r="B24">
-        <v>-0.24</v>
+        <v>-0.23</v>
       </c>
       <c r="C24">
-        <v>-0.84</v>
+        <v>-0.8</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
-        <v>384.15390468291196</v>
+        <f>5.67*10^-8*(B24+$E$1+273.14)^4</f>
+        <v>384.2074667588796</v>
       </c>
       <c r="E24">
-        <f t="shared" si="1"/>
-        <v>311.72642883331054</v>
+        <f>5.67*10^-8*(C24+$E$2+273.14)^4</f>
+        <v>311.90963566282767</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -5285,18 +5280,18 @@
         <v>1896</v>
       </c>
       <c r="B25">
-        <v>-0.15</v>
+        <v>-0.14000000000000001</v>
       </c>
       <c r="C25">
-        <v>-1.06</v>
+        <v>-1.02</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
-        <v>384.63616503082426</v>
+        <f>5.67*10^-8*(B25+$E$1+273.14)^4</f>
+        <v>384.68977752870001</v>
       </c>
       <c r="E25">
-        <f t="shared" si="1"/>
-        <v>310.72023349998278</v>
+        <f>5.67*10^-8*(C25+$E$2+273.14)^4</f>
+        <v>310.90299666451727</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -5304,18 +5299,18 @@
         <v>1897</v>
       </c>
       <c r="B26">
-        <v>-0.13</v>
+        <v>-0.12</v>
       </c>
       <c r="C26">
-        <v>-0.63</v>
+        <v>-0.6</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
-        <v>384.74339563096243</v>
+        <f>5.67*10^-8*(B26+$E$1+273.14)^4</f>
+        <v>384.79701933800214</v>
       </c>
       <c r="E26">
-        <f t="shared" si="1"/>
-        <v>312.68916576879064</v>
+        <f>5.67*10^-8*(C26+$E$2+273.14)^4</f>
+        <v>312.82688143621107</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -5323,18 +5318,18 @@
         <v>1898</v>
       </c>
       <c r="B27">
-        <v>-0.3</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="C27">
-        <v>-1.51</v>
+        <v>-1.49</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
-        <v>383.83264982356309</v>
+        <f>5.67*10^-8*(B27+$E$1+273.14)^4</f>
+        <v>383.93971237995703</v>
       </c>
       <c r="E27">
-        <f t="shared" si="1"/>
-        <v>308.66969543087725</v>
+        <f>5.67*10^-8*(C27+$E$2+273.14)^4</f>
+        <v>308.76061433907716</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -5342,18 +5337,18 @@
         <v>1899</v>
       </c>
       <c r="B28">
-        <v>-0.2</v>
+        <v>-0.18</v>
       </c>
       <c r="C28">
-        <v>-1.43</v>
+        <v>-1.42</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
-        <v>384.36818659357857</v>
+        <f>5.67*10^-8*(B28+$E$1+273.14)^4</f>
+        <v>384.47536115961219</v>
       </c>
       <c r="E28">
-        <f t="shared" si="1"/>
-        <v>309.03349157770413</v>
+        <f>5.67*10^-8*(C28+$E$2+273.14)^4</f>
+        <v>309.07898869631936</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -5361,18 +5356,18 @@
         <v>1900</v>
       </c>
       <c r="B29">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
       <c r="C29">
-        <v>-0.76</v>
+        <v>-0.75</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
-        <v>384.90428356797594</v>
+        <f>5.67*10^-8*(B29+$E$1+273.14)^4</f>
+        <v>384.95792409169127</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
-        <v>312.09292323576784</v>
+        <f>5.67*10^-8*(C29+$E$2+273.14)^4</f>
+        <v>312.13875774794229</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -5380,18 +5375,18 @@
         <v>1901</v>
       </c>
       <c r="B30">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
       <c r="C30">
-        <v>-0.76</v>
+        <v>-0.78</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
-        <v>384.52895684667084</v>
+        <f>5.67*10^-8*(B30+$E$1+273.14)^4</f>
+        <v>384.58255813694461</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
-        <v>312.09292323576784</v>
+        <f>5.67*10^-8*(C30+$E$2+273.14)^4</f>
+        <v>312.00126935488771</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -5399,18 +5394,18 @@
         <v>1902</v>
       </c>
       <c r="B31">
-        <v>-0.3</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="C31">
-        <v>-1.69</v>
+        <v>-1.52</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
-        <v>383.83264982356309</v>
+        <f>5.67*10^-8*(B31+$E$1+273.14)^4</f>
+        <v>383.8861783024949</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
-        <v>307.85232853569312</v>
+        <f>5.67*10^-8*(C31+$E$2+273.14)^4</f>
+        <v>308.62424350724052</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -5418,18 +5413,18 @@
         <v>1903</v>
       </c>
       <c r="B32">
-        <v>-0.39</v>
+        <v>-0.38</v>
       </c>
       <c r="C32">
-        <v>-0.45</v>
+        <v>-0.42</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
-        <v>383.35114538262775</v>
+        <f>5.67*10^-8*(B32+$E$1+273.14)^4</f>
+        <v>383.40462349235258</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
-        <v>313.51614224722954</v>
+        <f>5.67*10^-8*(C32+$E$2+273.14)^4</f>
+        <v>313.6541309743302</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -5437,18 +5432,18 @@
         <v>1904</v>
       </c>
       <c r="B33">
-        <v>-0.48</v>
+        <v>-0.46</v>
       </c>
       <c r="C33">
-        <v>-0.33</v>
+        <v>-0.23</v>
       </c>
       <c r="D33">
-        <f t="shared" si="0"/>
-        <v>382.87009410650859</v>
+        <f>5.67*10^-8*(B33+$E$1+273.14)^4</f>
+        <v>382.97695524226617</v>
       </c>
       <c r="E33">
-        <f t="shared" si="1"/>
-        <v>314.06837046577078</v>
+        <f>5.67*10^-8*(C33+$E$2+273.14)^4</f>
+        <v>314.52911764936545</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -5456,17 +5451,17 @@
         <v>1905</v>
       </c>
       <c r="B34">
-        <v>-0.27</v>
+        <v>-0.26</v>
       </c>
       <c r="C34">
         <v>-0.15</v>
       </c>
       <c r="D34">
-        <f t="shared" si="0"/>
-        <v>383.9932520563392</v>
+        <f>5.67*10^-8*(B34+$E$1+273.14)^4</f>
+        <v>384.0467973320321</v>
       </c>
       <c r="E34">
-        <f t="shared" si="1"/>
+        <f>5.67*10^-8*(C34+$E$2+273.14)^4</f>
         <v>314.89808024635863</v>
       </c>
     </row>
@@ -5475,18 +5470,18 @@
         <v>1906</v>
       </c>
       <c r="B35">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
       <c r="C35">
-        <v>-0.28000000000000003</v>
+        <v>-0.27</v>
       </c>
       <c r="D35">
-        <f t="shared" si="0"/>
-        <v>384.2074667588796</v>
+        <f>5.67*10^-8*(B35+$E$1+273.14)^4</f>
+        <v>384.26103443571941</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
-        <v>314.29868073564893</v>
+        <f>5.67*10^-8*(C35+$E$2+273.14)^4</f>
+        <v>314.34475798539989</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -5494,18 +5489,18 @@
         <v>1907</v>
       </c>
       <c r="B36">
-        <v>-0.41</v>
+        <v>-0.4</v>
       </c>
       <c r="C36">
-        <v>-0.59</v>
+        <v>-0.57999999999999996</v>
       </c>
       <c r="D36">
-        <f t="shared" si="0"/>
-        <v>383.24420594666913</v>
+        <f>5.67*10^-8*(B36+$E$1+273.14)^4</f>
+        <v>383.29767286753008</v>
       </c>
       <c r="E36">
-        <f t="shared" si="1"/>
-        <v>312.87279676594761</v>
+        <f>5.67*10^-8*(C36+$E$2+273.14)^4</f>
+        <v>312.91871714993346</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -5513,17 +5508,17 @@
         <v>1908</v>
       </c>
       <c r="B37">
-        <v>-0.43</v>
+        <v>-0.42</v>
       </c>
       <c r="C37">
         <v>-0.28999999999999998</v>
       </c>
       <c r="D37">
-        <f t="shared" si="0"/>
-        <v>383.13728888609842</v>
+        <f>5.67*10^-8*(B37+$E$1+273.14)^4</f>
+        <v>383.19074461965545</v>
       </c>
       <c r="E37">
-        <f t="shared" si="1"/>
+        <f>5.67*10^-8*(C37+$E$2+273.14)^4</f>
         <v>314.25260855165118</v>
       </c>
     </row>
@@ -5532,18 +5527,18 @@
         <v>1909</v>
       </c>
       <c r="B38">
-        <v>-0.5</v>
+        <v>-0.48</v>
       </c>
       <c r="C38">
-        <v>-0.78</v>
+        <v>-0.77</v>
       </c>
       <c r="D38">
-        <f t="shared" si="0"/>
-        <v>382.76325533521504</v>
+        <f>5.67*10^-8*(B38+$E$1+273.14)^4</f>
+        <v>382.87009410650859</v>
       </c>
       <c r="E38">
-        <f t="shared" si="1"/>
-        <v>312.00126935488771</v>
+        <f>5.67*10^-8*(C38+$E$2+273.14)^4</f>
+        <v>312.04709377153983</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -5551,18 +5546,18 @@
         <v>1910</v>
       </c>
       <c r="B39">
-        <v>-0.45</v>
+        <v>-0.43</v>
       </c>
       <c r="C39">
-        <v>-0.82</v>
+        <v>-0.63</v>
       </c>
       <c r="D39">
-        <f t="shared" si="0"/>
-        <v>383.0303941977939</v>
+        <f>5.67*10^-8*(B39+$E$1+273.14)^4</f>
+        <v>383.13728888609842</v>
       </c>
       <c r="E39">
-        <f t="shared" si="1"/>
-        <v>311.81802215662361</v>
+        <f>5.67*10^-8*(C39+$E$2+273.14)^4</f>
+        <v>312.68916576879064</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -5570,18 +5565,18 @@
         <v>1911</v>
       </c>
       <c r="B40">
-        <v>-0.45</v>
+        <v>-0.44</v>
       </c>
       <c r="C40">
-        <v>-0.39</v>
+        <v>-0.4</v>
       </c>
       <c r="D40">
-        <f t="shared" si="0"/>
-        <v>383.0303941977939</v>
+        <f>5.67*10^-8*(B40+$E$1+273.14)^4</f>
+        <v>383.08383874560803</v>
       </c>
       <c r="E40">
-        <f t="shared" si="1"/>
-        <v>313.79216524644022</v>
+        <f>5.67*10^-8*(C40+$E$2+273.14)^4</f>
+        <v>313.74614876122854</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -5589,17 +5584,17 @@
         <v>1912</v>
       </c>
       <c r="B41">
-        <v>-0.37</v>
+        <v>-0.36</v>
       </c>
       <c r="C41">
         <v>-0.66</v>
       </c>
       <c r="D41">
-        <f t="shared" ref="D41:D72" si="2">5.67*10^-8*(B41+$E$1+273.14)^4</f>
-        <v>383.4581071970951</v>
+        <f>5.67*10^-8*(B41+$E$1+273.14)^4</f>
+        <v>383.51159649724525</v>
       </c>
       <c r="E41">
-        <f t="shared" ref="E41:E72" si="3">5.67*10^-8*(C41+$E$2+273.14)^4</f>
+        <f>5.67*10^-8*(C41+$E$2+273.14)^4</f>
         <v>312.55149557626464</v>
       </c>
     </row>
@@ -5608,17 +5603,17 @@
         <v>1913</v>
       </c>
       <c r="B42">
-        <v>-0.37</v>
+        <v>-0.35</v>
       </c>
       <c r="C42">
         <v>-0.78</v>
       </c>
       <c r="D42">
-        <f t="shared" si="2"/>
-        <v>383.4581071970951</v>
+        <f>5.67*10^-8*(B42+$E$1+273.14)^4</f>
+        <v>383.56509139319331</v>
       </c>
       <c r="E42">
-        <f t="shared" si="3"/>
+        <f>5.67*10^-8*(C42+$E$2+273.14)^4</f>
         <v>312.00126935488771</v>
       </c>
     </row>
@@ -5627,18 +5622,18 @@
         <v>1914</v>
       </c>
       <c r="B43">
-        <v>-0.18</v>
+        <v>-0.16</v>
       </c>
       <c r="C43">
-        <v>-0.5</v>
+        <v>-0.49</v>
       </c>
       <c r="D43">
-        <f t="shared" si="2"/>
-        <v>384.47536115961219</v>
+        <f>5.67*10^-8*(B43+$E$1+273.14)^4</f>
+        <v>384.58255813694461</v>
       </c>
       <c r="E43">
-        <f t="shared" si="3"/>
-        <v>313.28626221931233</v>
+        <f>5.67*10^-8*(C43+$E$2+273.14)^4</f>
+        <v>313.33222810823565</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -5649,15 +5644,15 @@
         <v>-0.15</v>
       </c>
       <c r="C44">
-        <v>-0.77</v>
+        <v>-0.96</v>
       </c>
       <c r="D44">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B44+$E$1+273.14)^4</f>
         <v>384.63616503082426</v>
       </c>
       <c r="E44">
-        <f t="shared" si="3"/>
-        <v>312.04709377153983</v>
+        <f>5.67*10^-8*(C44+$E$2+273.14)^4</f>
+        <v>311.17729256814567</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -5665,18 +5660,18 @@
         <v>1916</v>
       </c>
       <c r="B45">
-        <v>-0.38</v>
+        <v>-0.36</v>
       </c>
       <c r="C45">
-        <v>-0.64</v>
+        <v>-0.55000000000000004</v>
       </c>
       <c r="D45">
-        <f t="shared" si="2"/>
-        <v>383.40462349235258</v>
+        <f>5.67*10^-8*(B45+$E$1+273.14)^4</f>
+        <v>383.51159649724525</v>
       </c>
       <c r="E45">
-        <f t="shared" si="3"/>
-        <v>312.64327065234374</v>
+        <f>5.67*10^-8*(C45+$E$2+273.14)^4</f>
+        <v>313.05650863109679</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -5687,15 +5682,15 @@
         <v>-0.48</v>
       </c>
       <c r="C46">
-        <v>-1.1200000000000001</v>
+        <v>-1.33</v>
       </c>
       <c r="D46">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B46+$E$1+273.14)^4</f>
         <v>382.87009410650859</v>
       </c>
       <c r="E46">
-        <f t="shared" si="3"/>
-        <v>310.44623985076419</v>
+        <f>5.67*10^-8*(C46+$E$2+273.14)^4</f>
+        <v>309.48868886630936</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -5703,18 +5698,18 @@
         <v>1918</v>
       </c>
       <c r="B47">
-        <v>-0.32</v>
+        <v>-0.31</v>
       </c>
       <c r="C47">
-        <v>-1.25</v>
+        <v>-1.2</v>
       </c>
       <c r="D47">
-        <f t="shared" si="2"/>
-        <v>383.72560965972832</v>
+        <f>5.67*10^-8*(B47+$E$1+273.14)^4</f>
+        <v>383.77912694277103</v>
       </c>
       <c r="E47">
-        <f t="shared" si="3"/>
-        <v>309.85320861201268</v>
+        <f>5.67*10^-8*(C47+$E$2+273.14)^4</f>
+        <v>310.08119690957619</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -5725,15 +5720,15 @@
         <v>-0.28999999999999998</v>
       </c>
       <c r="C48">
-        <v>-0.74</v>
+        <v>-0.88</v>
       </c>
       <c r="D48">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B48+$E$1+273.14)^4</f>
         <v>383.8861783024949</v>
       </c>
       <c r="E48">
-        <f t="shared" si="3"/>
-        <v>312.18459730843387</v>
+        <f>5.67*10^-8*(C48+$E$2+273.14)^4</f>
+        <v>311.54330272349921</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -5741,18 +5736,18 @@
         <v>1920</v>
       </c>
       <c r="B49">
-        <v>-0.28999999999999998</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="C49">
-        <v>-0.12</v>
+        <v>-0.08</v>
       </c>
       <c r="D49">
-        <f t="shared" si="2"/>
-        <v>383.8861783024949</v>
+        <f>5.67*10^-8*(B49+$E$1+273.14)^4</f>
+        <v>383.93971237995703</v>
       </c>
       <c r="E49">
-        <f t="shared" si="3"/>
-        <v>315.03652487461358</v>
+        <f>5.67*10^-8*(C49+$E$2+273.14)^4</f>
+        <v>315.22118871776757</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -5760,18 +5755,18 @@
         <v>1921</v>
       </c>
       <c r="B50">
-        <v>-0.2</v>
+        <v>-0.19</v>
       </c>
       <c r="C50">
-        <v>-0.15</v>
+        <v>-0.13</v>
       </c>
       <c r="D50">
-        <f t="shared" si="2"/>
-        <v>384.36818659357857</v>
+        <f>5.67*10^-8*(B50+$E$1+273.14)^4</f>
+        <v>384.42177107537833</v>
       </c>
       <c r="E50">
-        <f t="shared" si="3"/>
-        <v>314.89808024635863</v>
+        <f>5.67*10^-8*(C50+$E$2+273.14)^4</f>
+        <v>314.9903715939945</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -5779,18 +5774,18 @@
         <v>1922</v>
       </c>
       <c r="B51">
-        <v>-0.3</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="C51">
-        <v>-0.27</v>
+        <v>-0.35</v>
       </c>
       <c r="D51">
-        <f t="shared" si="2"/>
-        <v>383.83264982356309</v>
+        <f>5.67*10^-8*(B51+$E$1+273.14)^4</f>
+        <v>383.8861783024949</v>
       </c>
       <c r="E51">
-        <f t="shared" si="3"/>
-        <v>314.34475798539989</v>
+        <f>5.67*10^-8*(C51+$E$2+273.14)^4</f>
+        <v>313.97628180769811</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -5801,15 +5796,15 @@
         <v>-0.27</v>
       </c>
       <c r="C52">
-        <v>0.28000000000000003</v>
+        <v>0.24</v>
       </c>
       <c r="D52">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B52+$E$1+273.14)^4</f>
         <v>383.9932520563392</v>
       </c>
       <c r="E52">
-        <f t="shared" si="3"/>
-        <v>316.8868188521655</v>
+        <f>5.67*10^-8*(C52+$E$2+273.14)^4</f>
+        <v>316.70142361426849</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -5820,15 +5815,15 @@
         <v>-0.27</v>
       </c>
       <c r="C53">
-        <v>0.45</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D53">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B53+$E$1+273.14)^4</f>
         <v>383.9932520563392</v>
       </c>
       <c r="E53">
-        <f t="shared" si="3"/>
-        <v>317.67565685347773</v>
+        <f>5.67*10^-8*(C53+$E$2+273.14)^4</f>
+        <v>316.8868188521655</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
@@ -5836,18 +5831,18 @@
         <v>1925</v>
       </c>
       <c r="B54">
-        <v>-0.23</v>
+        <v>-0.22</v>
       </c>
       <c r="C54">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.12</v>
       </c>
       <c r="D54">
-        <f t="shared" si="2"/>
-        <v>384.2074667588796</v>
+        <f>5.67*10^-8*(B54+$E$1+273.14)^4</f>
+        <v>384.26103443571941</v>
       </c>
       <c r="E54">
-        <f t="shared" si="3"/>
-        <v>315.26736736058308</v>
+        <f>5.67*10^-8*(C54+$E$2+273.14)^4</f>
+        <v>315.03652487461358</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -5858,15 +5853,15 @@
         <v>-0.1</v>
       </c>
       <c r="C55">
-        <v>0.47</v>
+        <v>0.44</v>
       </c>
       <c r="D55">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B55+$E$1+273.14)^4</f>
         <v>384.90428356797594</v>
       </c>
       <c r="E55">
-        <f t="shared" si="3"/>
-        <v>317.7685580538672</v>
+        <f>5.67*10^-8*(C55+$E$2+273.14)^4</f>
+        <v>317.62921389281217</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -5874,18 +5869,18 @@
         <v>1927</v>
       </c>
       <c r="B56">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
       <c r="C56">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="D56">
-        <f t="shared" si="2"/>
-        <v>384.26103443571941</v>
+        <f>5.67*10^-8*(B56+$E$1+273.14)^4</f>
+        <v>384.31460771382257</v>
       </c>
       <c r="E56">
-        <f t="shared" si="3"/>
-        <v>315.91440125226575</v>
+        <f>5.67*10^-8*(C56+$E$2+273.14)^4</f>
+        <v>315.86815154587384</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -5896,15 +5891,15 @@
         <v>-0.2</v>
       </c>
       <c r="C57">
-        <v>0.77</v>
+        <v>0.83</v>
       </c>
       <c r="D57">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B57+$E$1+273.14)^4</f>
         <v>384.36818659357857</v>
       </c>
       <c r="E57">
-        <f t="shared" si="3"/>
-        <v>319.16452267534032</v>
+        <f>5.67*10^-8*(C57+$E$2+273.14)^4</f>
+        <v>319.44426659779566</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
@@ -5915,15 +5910,15 @@
         <v>-0.36</v>
       </c>
       <c r="C58">
-        <v>0.28000000000000003</v>
+        <v>0.3</v>
       </c>
       <c r="D58">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B58+$E$1+273.14)^4</f>
         <v>383.51159649724525</v>
       </c>
       <c r="E58">
-        <f t="shared" si="3"/>
-        <v>316.8868188521655</v>
+        <f>5.67*10^-8*(C58+$E$2+273.14)^4</f>
+        <v>316.9795469890347</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -5934,15 +5929,15 @@
         <v>-0.15</v>
       </c>
       <c r="C59">
-        <v>0.74</v>
+        <v>0.76</v>
       </c>
       <c r="D59">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B59+$E$1+273.14)^4</f>
         <v>384.63616503082426</v>
       </c>
       <c r="E59">
-        <f t="shared" si="3"/>
-        <v>319.02471963415906</v>
+        <f>5.67*10^-8*(C59+$E$2+273.14)^4</f>
+        <v>319.11791655729439</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -5953,15 +5948,15 @@
         <v>-0.08</v>
       </c>
       <c r="C60">
-        <v>0.74</v>
+        <v>0.72</v>
       </c>
       <c r="D60">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B60+$E$1+273.14)^4</f>
         <v>385.01157022174618</v>
       </c>
       <c r="E60">
-        <f t="shared" si="3"/>
-        <v>319.02471963415906</v>
+        <f>5.67*10^-8*(C60+$E$2+273.14)^4</f>
+        <v>318.93154312581487</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -5972,15 +5967,15 @@
         <v>-0.15</v>
       </c>
       <c r="C61">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
       <c r="D61">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B61+$E$1+273.14)^4</f>
         <v>384.63616503082426</v>
       </c>
       <c r="E61">
-        <f t="shared" si="3"/>
-        <v>318.5125013913663</v>
+        <f>5.67*10^-8*(C61+$E$2+273.14)^4</f>
+        <v>318.60558607004424</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -5988,18 +5983,18 @@
         <v>1933</v>
       </c>
       <c r="B62">
-        <v>-0.28999999999999998</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="C62">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="D62">
-        <f t="shared" si="2"/>
-        <v>383.8861783024949</v>
+        <f>5.67*10^-8*(B62+$E$1+273.14)^4</f>
+        <v>383.93971237995703</v>
       </c>
       <c r="E62">
-        <f t="shared" si="3"/>
-        <v>316.1920061575405</v>
+        <f>5.67*10^-8*(C62+$E$2+273.14)^4</f>
+        <v>316.05318084547457</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -6010,15 +6005,15 @@
         <v>-0.12</v>
       </c>
       <c r="C63">
-        <v>1.04</v>
+        <v>1.01</v>
       </c>
       <c r="D63">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B63+$E$1+273.14)^4</f>
         <v>384.79701933800214</v>
       </c>
       <c r="E63">
-        <f t="shared" si="3"/>
-        <v>320.42481870436319</v>
+        <f>5.67*10^-8*(C63+$E$2+273.14)^4</f>
+        <v>320.28460181068391</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -6026,18 +6021,18 @@
         <v>1935</v>
       </c>
       <c r="B64">
-        <v>-0.2</v>
+        <v>-0.19</v>
       </c>
       <c r="C64">
-        <v>0.41</v>
+        <v>0.45</v>
       </c>
       <c r="D64">
-        <f t="shared" si="2"/>
-        <v>384.36818659357857</v>
+        <f>5.67*10^-8*(B64+$E$1+273.14)^4</f>
+        <v>384.42177107537833</v>
       </c>
       <c r="E64">
-        <f t="shared" si="3"/>
-        <v>317.48991556446401</v>
+        <f>5.67*10^-8*(C64+$E$2+273.14)^4</f>
+        <v>317.67565685347773</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
@@ -6045,18 +6040,18 @@
         <v>1936</v>
       </c>
       <c r="B65">
-        <v>-0.14000000000000001</v>
+        <v>-0.13</v>
       </c>
       <c r="C65">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
       <c r="D65">
-        <f t="shared" si="2"/>
-        <v>384.68977752870001</v>
+        <f>5.67*10^-8*(B65+$E$1+273.14)^4</f>
+        <v>384.74339563096243</v>
       </c>
       <c r="E65">
-        <f t="shared" si="3"/>
-        <v>318.5125013913663</v>
+        <f>5.67*10^-8*(C65+$E$2+273.14)^4</f>
+        <v>318.3729126194097</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
@@ -6064,18 +6059,18 @@
         <v>1937</v>
       </c>
       <c r="B66">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="C66">
-        <v>1.44</v>
+        <v>1.45</v>
       </c>
       <c r="D66">
-        <f t="shared" si="2"/>
-        <v>385.33356475708479</v>
+        <f>5.67*10^-8*(B66+$E$1+273.14)^4</f>
+        <v>385.38725014245563</v>
       </c>
       <c r="E66">
-        <f t="shared" si="3"/>
-        <v>322.2987800464457</v>
+        <f>5.67*10^-8*(C66+$E$2+273.14)^4</f>
+        <v>322.34573414176174</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -6086,15 +6081,15 @@
         <v>0</v>
       </c>
       <c r="C67">
-        <v>1.88</v>
+        <v>1.84</v>
       </c>
       <c r="D67">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B67+$E$1+273.14)^4</f>
         <v>385.44094113729142</v>
       </c>
       <c r="E67">
-        <f t="shared" si="3"/>
-        <v>324.3696183540489</v>
+        <f>5.67*10^-8*(C67+$E$2+273.14)^4</f>
+        <v>324.18094910305086</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -6102,18 +6097,18 @@
         <v>1939</v>
       </c>
       <c r="B68">
-        <v>-0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="C68">
-        <v>0.61</v>
+        <v>0.62</v>
       </c>
       <c r="D68">
-        <f t="shared" si="2"/>
-        <v>385.33356475708479</v>
+        <f>5.67*10^-8*(B68+$E$1+273.14)^4</f>
+        <v>385.38725014245563</v>
       </c>
       <c r="E68">
-        <f t="shared" si="3"/>
-        <v>318.41943711108399</v>
+        <f>5.67*10^-8*(C68+$E$2+273.14)^4</f>
+        <v>318.46596670161199</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
@@ -6127,11 +6122,11 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="D69">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B69+$E$1+273.14)^4</f>
         <v>386.1932042776611</v>
       </c>
       <c r="E69">
-        <f t="shared" si="3"/>
+        <f>5.67*10^-8*(C69+$E$2+273.14)^4</f>
         <v>320.89254087405959</v>
       </c>
     </row>
@@ -6140,18 +6135,18 @@
         <v>1941</v>
       </c>
       <c r="B70">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="C70">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <f t="shared" si="2"/>
-        <v>386.46213635729197</v>
+        <f>5.67*10^-8*(B70+$E$1+273.14)^4</f>
+        <v>386.51593962350103</v>
       </c>
       <c r="E70">
-        <f t="shared" si="3"/>
-        <v>315.72943289552609</v>
+        <f>5.67*10^-8*(C70+$E$2+273.14)^4</f>
+        <v>315.59075994061396</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
@@ -6162,15 +6157,15 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C71">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="D71">
-        <f t="shared" si="2"/>
+        <f>5.67*10^-8*(B71+$E$1+273.14)^4</f>
         <v>385.81693519898806</v>
       </c>
       <c r="E71">
-        <f t="shared" si="3"/>
-        <v>320.05100925822074</v>
+        <f>5.67*10^-8*(C71+$E$2+273.14)^4</f>
+        <v>319.95760802314891</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
@@ -6178,18 +6173,18 @@
         <v>1943</v>
       </c>
       <c r="B72">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="C72">
-        <v>1.51</v>
+        <v>1.49</v>
       </c>
       <c r="D72">
-        <f t="shared" si="2"/>
-        <v>385.92441258121801</v>
+        <f>5.67*10^-8*(B72+$E$1+273.14)^4</f>
+        <v>385.97815969219738</v>
       </c>
       <c r="E72">
-        <f t="shared" si="3"/>
-        <v>322.62756646079947</v>
+        <f>5.67*10^-8*(C72+$E$2+273.14)^4</f>
+        <v>322.5336018286975</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
@@ -6203,11 +6198,11 @@
         <v>1.21</v>
       </c>
       <c r="D73">
-        <f t="shared" ref="D73:D104" si="4">5.67*10^-8*(B73+$E$1+273.14)^4</f>
+        <f>5.67*10^-8*(B73+$E$1+273.14)^4</f>
         <v>386.51593962350103</v>
       </c>
       <c r="E73">
-        <f t="shared" ref="E73:E104" si="5">5.67*10^-8*(C73+$E$2+273.14)^4</f>
+        <f>5.67*10^-8*(C73+$E$2+273.14)^4</f>
         <v>321.22025092832246</v>
       </c>
     </row>
@@ -6219,15 +6214,15 @@
         <v>0.1</v>
       </c>
       <c r="C74">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="D74">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B74+$E$1+273.14)^4</f>
         <v>385.97815969219738</v>
       </c>
       <c r="E74">
-        <f t="shared" si="5"/>
-        <v>319.72419437414351</v>
+        <f>5.67*10^-8*(C74+$E$2+273.14)^4</f>
+        <v>319.63086468217966</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
@@ -6241,11 +6236,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D75">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B75+$E$1+273.14)^4</f>
         <v>385.06522195853137</v>
       </c>
       <c r="E75">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C75+$E$2+273.14)^4</f>
         <v>315.91440125226575</v>
       </c>
     </row>
@@ -6260,11 +6255,11 @@
         <v>1.34</v>
       </c>
       <c r="D76">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B76+$E$1+273.14)^4</f>
         <v>385.38725014245563</v>
       </c>
       <c r="E76">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C76+$E$2+273.14)^4</f>
         <v>321.82952117172454</v>
       </c>
     </row>
@@ -6279,11 +6274,11 @@
         <v>-0.08</v>
       </c>
       <c r="D77">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B77+$E$1+273.14)^4</f>
         <v>384.90428356797594</v>
       </c>
       <c r="E77">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C77+$E$2+273.14)^4</f>
         <v>315.22118871776757</v>
       </c>
     </row>
@@ -6295,15 +6290,15 @@
         <v>-0.11</v>
       </c>
       <c r="C78">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="D78">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B78+$E$1+273.14)^4</f>
         <v>384.85064865020979</v>
       </c>
       <c r="E78">
-        <f t="shared" si="5"/>
-        <v>316.51610973765031</v>
+        <f>5.67*10^-8*(C78+$E$2+273.14)^4</f>
+        <v>316.56243058048676</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -6311,18 +6306,18 @@
         <v>1950</v>
       </c>
       <c r="B79">
-        <v>-0.18</v>
+        <v>-0.17</v>
       </c>
       <c r="C79">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="D79">
-        <f t="shared" si="4"/>
-        <v>384.47536115961219</v>
+        <f>5.67*10^-8*(B79+$E$1+273.14)^4</f>
+        <v>384.52895684667084</v>
       </c>
       <c r="E79">
-        <f t="shared" si="5"/>
-        <v>317.02591868825147</v>
+        <f>5.67*10^-8*(C79+$E$2+273.14)^4</f>
+        <v>317.1186773501102</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
@@ -6330,18 +6325,18 @@
         <v>1951</v>
       </c>
       <c r="B80">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.06</v>
       </c>
       <c r="C80">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="D80">
-        <f t="shared" si="4"/>
-        <v>385.06522195853137</v>
+        <f>5.67*10^-8*(B80+$E$1+273.14)^4</f>
+        <v>385.11887930243745</v>
       </c>
       <c r="E80">
-        <f t="shared" si="5"/>
-        <v>315.82190691786786</v>
+        <f>5.67*10^-8*(C80+$E$2+273.14)^4</f>
+        <v>315.86815154587384</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -6352,15 +6347,15 @@
         <v>0.01</v>
       </c>
       <c r="C81">
-        <v>0.5</v>
+        <v>0.49</v>
       </c>
       <c r="D81">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B81+$E$1+273.14)^4</f>
         <v>385.49463774198318</v>
       </c>
       <c r="E81">
-        <f t="shared" si="5"/>
-        <v>317.90794805768098</v>
+        <f>5.67*10^-8*(C81+$E$2+273.14)^4</f>
+        <v>317.86147962881603</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -6371,15 +6366,15 @@
         <v>0.09</v>
       </c>
       <c r="C82">
-        <v>1.1399999999999999</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D82">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B82+$E$1+273.14)^4</f>
         <v>385.92441258121801</v>
       </c>
       <c r="E82">
-        <f t="shared" si="5"/>
-        <v>320.89254087405959</v>
+        <f>5.67*10^-8*(C82+$E$2+273.14)^4</f>
+        <v>320.79895550313137</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -6390,15 +6385,15 @@
         <v>-0.13</v>
       </c>
       <c r="C83">
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
       <c r="D83">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B83+$E$1+273.14)^4</f>
         <v>384.74339563096243</v>
       </c>
       <c r="E83">
-        <f t="shared" si="5"/>
-        <v>320.47156789819479</v>
+        <f>5.67*10^-8*(C83+$E$2+273.14)^4</f>
+        <v>320.51832220728426</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -6409,15 +6404,15 @@
         <v>-0.14000000000000001</v>
       </c>
       <c r="C84">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="D84">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B84+$E$1+273.14)^4</f>
         <v>384.68977752870001</v>
       </c>
       <c r="E84">
-        <f t="shared" si="5"/>
-        <v>314.89808024635863</v>
+        <f>5.67*10^-8*(C84+$E$2+273.14)^4</f>
+        <v>314.85194217859879</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -6428,15 +6423,15 @@
         <v>-0.18</v>
       </c>
       <c r="C85">
-        <v>0.3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D85">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B85+$E$1+273.14)^4</f>
         <v>384.47536115961219</v>
       </c>
       <c r="E85">
-        <f t="shared" si="5"/>
-        <v>316.9795469890347</v>
+        <f>5.67*10^-8*(C85+$E$2+273.14)^4</f>
+        <v>316.93318037713016</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -6450,11 +6445,11 @@
         <v>0.08</v>
       </c>
       <c r="D86">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B86+$E$1+273.14)^4</f>
         <v>385.7094802671233</v>
       </c>
       <c r="E86">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C86+$E$2+273.14)^4</f>
         <v>315.96065603741522</v>
       </c>
     </row>
@@ -6466,15 +6461,15 @@
         <v>0.06</v>
       </c>
       <c r="C87">
-        <v>-0.11</v>
+        <v>-0.09</v>
       </c>
       <c r="D87">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B87+$E$1+273.14)^4</f>
         <v>385.7632049269555</v>
       </c>
       <c r="E87">
-        <f t="shared" si="5"/>
-        <v>315.08268322692891</v>
+        <f>5.67*10^-8*(C87+$E$2+273.14)^4</f>
+        <v>315.17501514813443</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -6482,18 +6477,18 @@
         <v>1959</v>
       </c>
       <c r="B88">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="C88">
-        <v>0.56999999999999995</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="D88">
-        <f t="shared" si="4"/>
-        <v>385.54833995692138</v>
+        <f>5.67*10^-8*(B88+$E$1+273.14)^4</f>
+        <v>385.60204778249698</v>
       </c>
       <c r="E88">
-        <f t="shared" si="5"/>
-        <v>318.2333697337848</v>
+        <f>5.67*10^-8*(C88+$E$2+273.14)^4</f>
+        <v>318.18686563380078</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -6504,15 +6499,15 @@
         <v>-0.03</v>
       </c>
       <c r="C89">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
       <c r="D89">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B89+$E$1+273.14)^4</f>
         <v>385.27988498078827</v>
       </c>
       <c r="E89">
-        <f t="shared" si="5"/>
-        <v>317.35066305877109</v>
+        <f>5.67*10^-8*(C89+$E$2+273.14)^4</f>
+        <v>317.30425573794872</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -6523,15 +6518,15 @@
         <v>0.06</v>
       </c>
       <c r="C90">
-        <v>-0.22</v>
+        <v>-0.21</v>
       </c>
       <c r="D90">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B90+$E$1+273.14)^4</f>
         <v>385.7632049269555</v>
       </c>
       <c r="E90">
-        <f t="shared" si="5"/>
-        <v>314.57522023345405</v>
+        <f>5.67*10^-8*(C90+$E$2+273.14)^4</f>
+        <v>314.62132788552441</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -6545,11 +6540,11 @@
         <v>0.32</v>
       </c>
       <c r="D91">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B91+$E$1+273.14)^4</f>
         <v>385.60204778249698</v>
       </c>
       <c r="E91">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C91+$E$2+273.14)^4</f>
         <v>317.07229547515254</v>
       </c>
     </row>
@@ -6564,11 +6559,11 @@
         <v>-0.44</v>
       </c>
       <c r="D92">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B92+$E$1+273.14)^4</f>
         <v>385.7632049269555</v>
       </c>
       <c r="E92">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C92+$E$2+273.14)^4</f>
         <v>313.56213342965839</v>
       </c>
     </row>
@@ -6580,15 +6575,15 @@
         <v>-0.2</v>
       </c>
       <c r="C93">
-        <v>-0.71</v>
+        <v>-0.73</v>
       </c>
       <c r="D93">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B93+$E$1+273.14)^4</f>
         <v>384.36818659357857</v>
       </c>
       <c r="E93">
-        <f t="shared" si="5"/>
-        <v>312.32214628351784</v>
+        <f>5.67*10^-8*(C93+$E$2+273.14)^4</f>
+        <v>312.23044191761312</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -6602,11 +6597,11 @@
         <v>-0.17</v>
       </c>
       <c r="D94">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B94+$E$1+273.14)^4</f>
         <v>384.85064865020979</v>
       </c>
       <c r="E94">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C94+$E$2+273.14)^4</f>
         <v>314.80580918104931</v>
       </c>
     </row>
@@ -6621,11 +6616,11 @@
         <v>-0.78</v>
       </c>
       <c r="D95">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B95+$E$1+273.14)^4</f>
         <v>385.11887930243745</v>
       </c>
       <c r="E95">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C95+$E$2+273.14)^4</f>
         <v>312.00126935488771</v>
       </c>
     </row>
@@ -6640,11 +6635,11 @@
         <v>0.26</v>
       </c>
       <c r="D96">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B96+$E$1+273.14)^4</f>
         <v>385.33356475708479</v>
       </c>
       <c r="E96">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C96+$E$2+273.14)^4</f>
         <v>316.79411106156897</v>
       </c>
     </row>
@@ -6659,11 +6654,11 @@
         <v>-0.5</v>
       </c>
       <c r="D97">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B97+$E$1+273.14)^4</f>
         <v>385.01157022174618</v>
       </c>
       <c r="E97">
-        <f t="shared" si="5"/>
+        <f>5.67*10^-8*(C97+$E$2+273.14)^4</f>
         <v>313.28626221931233</v>
       </c>
     </row>
@@ -6675,15 +6670,15 @@
         <v>0.05</v>
       </c>
       <c r="C98">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
       <c r="D98">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B98+$E$1+273.14)^4</f>
         <v>385.7094802671233</v>
       </c>
       <c r="E98">
-        <f t="shared" si="5"/>
-        <v>315.91440125226575</v>
+        <f>5.67*10^-8*(C98+$E$2+273.14)^4</f>
+        <v>315.86815154587384</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -6694,15 +6689,15 @@
         <v>0.02</v>
       </c>
       <c r="C99">
-        <v>-0.26</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="D99">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B99+$E$1+273.14)^4</f>
         <v>385.54833995692138</v>
       </c>
       <c r="E99">
-        <f t="shared" si="5"/>
-        <v>314.39084030127572</v>
+        <f>5.67*10^-8*(C99+$E$2+273.14)^4</f>
+        <v>314.29868073564893</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -6710,18 +6705,18 @@
         <v>1971</v>
       </c>
       <c r="B100">
-        <v>-0.08</v>
+        <v>-0.09</v>
       </c>
       <c r="C100">
-        <v>-0.04</v>
+        <v>-0.05</v>
       </c>
       <c r="D100">
-        <f t="shared" si="4"/>
-        <v>385.01157022174618</v>
+        <f>5.67*10^-8*(B100+$E$1+273.14)^4</f>
+        <v>384.95792409169127</v>
       </c>
       <c r="E100">
-        <f t="shared" si="5"/>
-        <v>315.40593373183998</v>
+        <f>5.67*10^-8*(C100+$E$2+273.14)^4</f>
+        <v>315.3597398672477</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -6732,15 +6727,15 @@
         <v>0</v>
       </c>
       <c r="C101">
-        <v>-0.16</v>
+        <v>-0.15</v>
       </c>
       <c r="D101">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B101+$E$1+273.14)^4</f>
         <v>385.44094113729142</v>
       </c>
       <c r="E101">
-        <f t="shared" si="5"/>
-        <v>314.85194217859879</v>
+        <f>5.67*10^-8*(C101+$E$2+273.14)^4</f>
+        <v>314.89808024635863</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -6751,15 +6746,15 @@
         <v>0.17</v>
       </c>
       <c r="C102">
-        <v>-0.08</v>
+        <v>-0.06</v>
       </c>
       <c r="D102">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B102+$E$1+273.14)^4</f>
         <v>386.35454667632962</v>
       </c>
       <c r="E102">
-        <f t="shared" si="5"/>
-        <v>315.22118871776757</v>
+        <f>5.67*10^-8*(C102+$E$2+273.14)^4</f>
+        <v>315.31355107695254</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -6770,15 +6765,15 @@
         <v>-0.06</v>
       </c>
       <c r="C103">
-        <v>-0.11</v>
+        <v>-0.12</v>
       </c>
       <c r="D103">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B103+$E$1+273.14)^4</f>
         <v>385.11887930243745</v>
       </c>
       <c r="E103">
-        <f t="shared" si="5"/>
-        <v>315.08268322692891</v>
+        <f>5.67*10^-8*(C103+$E$2+273.14)^4</f>
+        <v>315.03652487461358</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -6789,15 +6784,15 @@
         <v>-0.02</v>
       </c>
       <c r="C104">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.08</v>
       </c>
       <c r="D104">
-        <f t="shared" si="4"/>
+        <f>5.67*10^-8*(B104+$E$1+273.14)^4</f>
         <v>385.33356475708479</v>
       </c>
       <c r="E104">
-        <f t="shared" si="5"/>
-        <v>315.26736736058308</v>
+        <f>5.67*10^-8*(C104+$E$2+273.14)^4</f>
+        <v>315.22118871776757</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -6808,15 +6803,15 @@
         <v>-0.11</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D105">
-        <f t="shared" ref="D105:D136" si="6">5.67*10^-8*(B105+$E$1+273.14)^4</f>
+        <f>5.67*10^-8*(B105+$E$1+273.14)^4</f>
         <v>384.85064865020979</v>
       </c>
       <c r="E105">
-        <f t="shared" ref="E105:E136" si="7">5.67*10^-8*(C105+$E$2+273.14)^4</f>
-        <v>315.59075994061396</v>
+        <f>5.67*10^-8*(C105+$E$2+273.14)^4</f>
+        <v>315.63697918226694</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -6830,11 +6825,11 @@
         <v>0.02</v>
       </c>
       <c r="D106">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B106+$E$1+273.14)^4</f>
         <v>386.40833870836519</v>
       </c>
       <c r="E106">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C106+$E$2+273.14)^4</f>
         <v>315.68320350044701</v>
       </c>
     </row>
@@ -6843,18 +6838,18 @@
         <v>1978</v>
       </c>
       <c r="B107">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C107">
-        <v>-0.3</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="D107">
-        <f t="shared" si="6"/>
-        <v>385.7632049269555</v>
+        <f>5.67*10^-8*(B107+$E$1+273.14)^4</f>
+        <v>385.81693519898806</v>
       </c>
       <c r="E107">
-        <f t="shared" si="7"/>
-        <v>314.20654143303597</v>
+        <f>5.67*10^-8*(C107+$E$2+273.14)^4</f>
+        <v>314.25260855165118</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -6865,15 +6860,15 @@
         <v>0.16</v>
       </c>
       <c r="C108">
-        <v>-0.77</v>
+        <v>-0.75</v>
       </c>
       <c r="D108">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B108+$E$1+273.14)^4</f>
         <v>386.30076026079456</v>
       </c>
       <c r="E108">
-        <f t="shared" si="7"/>
-        <v>312.04709377153983</v>
+        <f>5.67*10^-8*(C108+$E$2+273.14)^4</f>
+        <v>312.13875774794229</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -6887,11 +6882,11 @@
         <v>0.15</v>
       </c>
       <c r="D109">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B109+$E$1+273.14)^4</f>
         <v>386.8388772055817</v>
       </c>
       <c r="E109">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C109+$E$2+273.14)^4</f>
         <v>316.28458176990767</v>
       </c>
     </row>
@@ -6906,11 +6901,11 @@
         <v>0.96</v>
       </c>
       <c r="D110">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B110+$E$1+273.14)^4</f>
         <v>387.21589343483623</v>
       </c>
       <c r="E110">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C110+$E$2+273.14)^4</f>
         <v>320.05100925822074</v>
       </c>
     </row>
@@ -6925,11 +6920,11 @@
         <v>-0.47</v>
       </c>
       <c r="D111">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B111+$E$1+273.14)^4</f>
         <v>386.13943470928126</v>
       </c>
       <c r="E111">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C111+$E$2+273.14)^4</f>
         <v>313.42417506033024</v>
       </c>
     </row>
@@ -6944,11 +6939,11 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D112">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B112+$E$1+273.14)^4</f>
         <v>387.10814640427151</v>
       </c>
       <c r="E112">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C112+$E$2+273.14)^4</f>
         <v>315.91440125226575</v>
       </c>
     </row>
@@ -6960,15 +6955,15 @@
         <v>0.16</v>
       </c>
       <c r="C113">
-        <v>0.54</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D113">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B113+$E$1+273.14)^4</f>
         <v>386.30076026079456</v>
       </c>
       <c r="E113">
-        <f t="shared" si="7"/>
-        <v>318.09387272443468</v>
+        <f>5.67*10^-8*(C113+$E$2+273.14)^4</f>
+        <v>318.14036663080833</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -6982,11 +6977,11 @@
         <v>0.48</v>
       </c>
       <c r="D114">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B114+$E$1+273.14)^4</f>
         <v>386.0319124169402</v>
       </c>
       <c r="E114">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C114+$E$2+273.14)^4</f>
         <v>317.81501629433546</v>
       </c>
     </row>
@@ -7001,11 +6996,11 @@
         <v>-0.15</v>
       </c>
       <c r="D115">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B115+$E$1+273.14)^4</f>
         <v>386.35454667632962</v>
       </c>
       <c r="E115">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C115+$E$2+273.14)^4</f>
         <v>314.89808024635863</v>
       </c>
     </row>
@@ -7017,15 +7012,15 @@
         <v>0.31</v>
       </c>
       <c r="C116">
-        <v>-0.52</v>
+        <v>-0.51</v>
       </c>
       <c r="D116">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B116+$E$1+273.14)^4</f>
         <v>387.10814640427151</v>
       </c>
       <c r="E116">
-        <f t="shared" si="7"/>
-        <v>313.19434561385918</v>
+        <f>5.67*10^-8*(C116+$E$2+273.14)^4</f>
+        <v>313.24030138797718</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -7033,17 +7028,17 @@
         <v>1988</v>
       </c>
       <c r="B117">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
       <c r="C117">
         <v>0.37</v>
       </c>
       <c r="D117">
-        <f t="shared" si="6"/>
-        <v>387.5392694852323</v>
+        <f>5.67*10^-8*(B117+$E$1+273.14)^4</f>
+        <v>387.48535941635276</v>
       </c>
       <c r="E117">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C117+$E$2+273.14)^4</f>
         <v>317.30425573794872</v>
       </c>
     </row>
@@ -7058,11 +7053,11 @@
         <v>0.12</v>
       </c>
       <c r="D118">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B118+$E$1+273.14)^4</f>
         <v>386.89271980371592</v>
       </c>
       <c r="E118">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C118+$E$2+273.14)^4</f>
         <v>316.14572597302583</v>
       </c>
     </row>
@@ -7077,11 +7072,11 @@
         <v>0.65</v>
       </c>
       <c r="D119">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B119+$E$1+273.14)^4</f>
         <v>387.80890421403086</v>
       </c>
       <c r="E119">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C119+$E$2+273.14)^4</f>
         <v>318.60558607004424</v>
       </c>
     </row>
@@ -7096,11 +7091,11 @@
         <v>0.67</v>
       </c>
       <c r="D120">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B120+$E$1+273.14)^4</f>
         <v>387.64710649869789</v>
       </c>
       <c r="E120">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C120+$E$2+273.14)^4</f>
         <v>318.6986911500984</v>
       </c>
     </row>
@@ -7115,11 +7110,11 @@
         <v>-0.28000000000000003</v>
       </c>
       <c r="D121">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B121+$E$1+273.14)^4</f>
         <v>386.62356300933067</v>
       </c>
       <c r="E121">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C121+$E$2+273.14)^4</f>
         <v>314.29868073564893</v>
       </c>
     </row>
@@ -7134,11 +7129,11 @@
         <v>0.46</v>
       </c>
       <c r="D122">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B122+$E$1+273.14)^4</f>
         <v>386.67738312973268</v>
       </c>
       <c r="E122">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C122+$E$2+273.14)^4</f>
         <v>317.72210490703856</v>
       </c>
     </row>
@@ -7153,11 +7148,11 @@
         <v>0.35</v>
       </c>
       <c r="D123">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B123+$E$1+273.14)^4</f>
         <v>387.16201710837066</v>
       </c>
       <c r="E123">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C123+$E$2+273.14)^4</f>
         <v>317.21145636568383</v>
       </c>
     </row>
@@ -7172,11 +7167,11 @@
         <v>1.26</v>
       </c>
       <c r="D124">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B124+$E$1+273.14)^4</f>
         <v>387.80890421403086</v>
       </c>
       <c r="E124">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C124+$E$2+273.14)^4</f>
         <v>321.45448316792823</v>
       </c>
     </row>
@@ -7191,11 +7186,11 @@
         <v>0.86</v>
       </c>
       <c r="D125">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B125+$E$1+273.14)^4</f>
         <v>387.26977538405936</v>
       </c>
       <c r="E125">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C125+$E$2+273.14)^4</f>
         <v>319.58420749919998</v>
       </c>
     </row>
@@ -7207,15 +7202,15 @@
         <v>0.46</v>
       </c>
       <c r="C126">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
       <c r="D126">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B126+$E$1+273.14)^4</f>
         <v>387.91679749224176</v>
       </c>
       <c r="E126">
-        <f t="shared" si="7"/>
-        <v>318.5125013913663</v>
+        <f>5.67*10^-8*(C126+$E$2+273.14)^4</f>
+        <v>318.46596670161199</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
@@ -7229,11 +7224,11 @@
         <v>0.95</v>
       </c>
       <c r="D127">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B127+$E$1+273.14)^4</f>
         <v>388.72671484522147</v>
       </c>
       <c r="E127">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C127+$E$2+273.14)^4</f>
         <v>320.0043060849211</v>
       </c>
     </row>
@@ -7245,15 +7240,15 @@
         <v>0.37</v>
       </c>
       <c r="C128">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="D128">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B128+$E$1+273.14)^4</f>
         <v>387.43145497218694</v>
       </c>
       <c r="E128">
-        <f t="shared" si="7"/>
-        <v>317.5827760246695</v>
+        <f>5.67*10^-8*(C128+$E$2+273.14)^4</f>
+        <v>317.62921389281217</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
@@ -7267,11 +7262,11 @@
         <v>0.92</v>
       </c>
       <c r="D129">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B129+$E$1+273.14)^4</f>
         <v>387.59318517921673</v>
       </c>
       <c r="E129">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C129+$E$2+273.14)^4</f>
         <v>319.86422723269442</v>
       </c>
     </row>
@@ -7286,11 +7281,11 @@
         <v>1.07</v>
       </c>
       <c r="D130">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B130+$E$1+273.14)^4</f>
         <v>388.3485957501664</v>
       </c>
       <c r="E130">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C130+$E$2+273.14)^4</f>
         <v>320.56508163200465</v>
       </c>
     </row>
@@ -7302,15 +7297,15 @@
         <v>0.63</v>
       </c>
       <c r="C131">
-        <v>1.27</v>
+        <v>1.28</v>
       </c>
       <c r="D131">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B131+$E$1+273.14)^4</f>
         <v>388.83479956995308</v>
       </c>
       <c r="E131">
-        <f t="shared" si="7"/>
-        <v>321.50134498364474</v>
+        <f>5.67*10^-8*(C131+$E$2+273.14)^4</f>
+        <v>321.54821192283077</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
@@ -7321,15 +7316,15 @@
         <v>0.62</v>
       </c>
       <c r="C132">
-        <v>1.36</v>
+        <v>1.35</v>
       </c>
       <c r="D132">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B132+$E$1+273.14)^4</f>
         <v>388.78075439053333</v>
       </c>
       <c r="E132">
-        <f t="shared" si="7"/>
-        <v>321.92333192604372</v>
+        <f>5.67*10^-8*(C132+$E$2+273.14)^4</f>
+        <v>321.87642398565549</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
@@ -7337,18 +7332,18 @@
         <v>2004</v>
       </c>
       <c r="B133">
-        <v>0.54</v>
+        <v>0.53</v>
       </c>
       <c r="C133">
-        <v>0.34</v>
+        <v>0.33</v>
       </c>
       <c r="D133">
-        <f t="shared" si="6"/>
-        <v>388.3485957501664</v>
+        <f>5.67*10^-8*(B133+$E$1+273.14)^4</f>
+        <v>388.29460126362119</v>
       </c>
       <c r="E133">
-        <f t="shared" si="7"/>
-        <v>317.16506431349643</v>
+        <f>5.67*10^-8*(C133+$E$2+273.14)^4</f>
+        <v>317.1186773501102</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
@@ -7356,17 +7351,17 @@
         <v>2005</v>
       </c>
       <c r="B134">
-        <v>0.68</v>
+        <v>0.67</v>
       </c>
       <c r="C134">
         <v>2.0699999999999998</v>
       </c>
       <c r="D134">
-        <f t="shared" si="6"/>
-        <v>389.10510999237562</v>
+        <f>5.67*10^-8*(B134+$E$1+273.14)^4</f>
+        <v>389.05103663654262</v>
       </c>
       <c r="E134">
-        <f t="shared" si="7"/>
+        <f>5.67*10^-8*(C134+$E$2+273.14)^4</f>
         <v>325.26692216598116</v>
       </c>
     </row>
@@ -7378,15 +7373,15 @@
         <v>0.64</v>
       </c>
       <c r="C135">
-        <v>2.04</v>
+        <v>2.0299999999999998</v>
       </c>
       <c r="D135">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B135+$E$1+273.14)^4</f>
         <v>388.8888503838723</v>
       </c>
       <c r="E135">
-        <f t="shared" si="7"/>
-        <v>325.12511900135144</v>
+        <f>5.67*10^-8*(C135+$E$2+273.14)^4</f>
+        <v>325.07786158483344</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
@@ -7397,15 +7392,15 @@
         <v>0.67</v>
       </c>
       <c r="C136">
-        <v>2.2200000000000002</v>
+        <v>2.27</v>
       </c>
       <c r="D136">
-        <f t="shared" si="6"/>
+        <f>5.67*10^-8*(B136+$E$1+273.14)^4</f>
         <v>389.05103663654262</v>
       </c>
       <c r="E136">
-        <f t="shared" si="7"/>
-        <v>325.97663389858718</v>
+        <f>5.67*10^-8*(C136+$E$2+273.14)^4</f>
+        <v>326.21346236396727</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
@@ -7419,11 +7414,11 @@
         <v>1.69</v>
       </c>
       <c r="D137">
-        <f t="shared" ref="D137:D153" si="8">5.67*10^-8*(B137+$E$1+273.14)^4</f>
+        <f>5.67*10^-8*(B137+$E$1+273.14)^4</f>
         <v>388.3485957501664</v>
       </c>
       <c r="E137">
-        <f t="shared" ref="E137:E153" si="9">5.67*10^-8*(C137+$E$2+273.14)^4</f>
+        <f>5.67*10^-8*(C137+$E$2+273.14)^4</f>
         <v>323.47417234698594</v>
       </c>
     </row>
@@ -7435,15 +7430,15 @@
         <v>0.66</v>
       </c>
       <c r="C138">
-        <v>1.68</v>
+        <v>1.67</v>
       </c>
       <c r="D138">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B138+$E$1+273.14)^4</f>
         <v>388.99696891677559</v>
       </c>
       <c r="E138">
-        <f t="shared" si="9"/>
-        <v>323.42709502386759</v>
+        <f>5.67*10^-8*(C138+$E$2+273.14)^4</f>
+        <v>323.38002283954052</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
@@ -7451,18 +7446,18 @@
         <v>2010</v>
       </c>
       <c r="B139">
-        <v>0.73</v>
+        <v>0.72</v>
       </c>
       <c r="C139">
-        <v>2.5</v>
+        <v>2.46</v>
       </c>
       <c r="D139">
-        <f t="shared" si="8"/>
-        <v>389.37556132623837</v>
+        <f>5.67*10^-8*(B139+$E$1+273.14)^4</f>
+        <v>389.32145978420073</v>
       </c>
       <c r="E139">
-        <f t="shared" si="9"/>
-        <v>327.30453583213392</v>
+        <f>5.67*10^-8*(C139+$E$2+273.14)^4</f>
+        <v>327.11458761176817</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
@@ -7473,15 +7468,15 @@
         <v>0.61</v>
       </c>
       <c r="C140">
-        <v>2.65</v>
+        <v>2.68</v>
       </c>
       <c r="D140">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B140+$E$1+273.14)^4</f>
         <v>388.72671484522147</v>
       </c>
       <c r="E140">
-        <f t="shared" si="9"/>
-        <v>328.0175785086895</v>
+        <f>5.67*10^-8*(C140+$E$2+273.14)^4</f>
+        <v>328.16032673200743</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
@@ -7492,15 +7487,15 @@
         <v>0.64</v>
       </c>
       <c r="C141">
-        <v>2.65</v>
+        <v>2.74</v>
       </c>
       <c r="D141">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B141+$E$1+273.14)^4</f>
         <v>388.8888503838723</v>
       </c>
       <c r="E141">
-        <f t="shared" si="9"/>
-        <v>328.0175785086895</v>
+        <f>5.67*10^-8*(C141+$E$2+273.14)^4</f>
+        <v>328.44596294771134</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
@@ -7514,11 +7509,11 @@
         <v>1.64</v>
       </c>
       <c r="D142">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B142+$E$1+273.14)^4</f>
         <v>389.10510999237562</v>
       </c>
       <c r="E142">
-        <f t="shared" si="9"/>
+        <f>5.67*10^-8*(C142+$E$2+273.14)^4</f>
         <v>323.23883711556692</v>
       </c>
     </row>
@@ -7527,18 +7522,18 @@
         <v>2014</v>
       </c>
       <c r="B143">
-        <v>0.75</v>
+        <v>0.74</v>
       </c>
       <c r="C143">
-        <v>2.2200000000000002</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D143">
-        <f t="shared" si="8"/>
-        <v>389.48378132595394</v>
+        <f>5.67*10^-8*(B143+$E$1+273.14)^4</f>
+        <v>389.42966850669217</v>
       </c>
       <c r="E143">
-        <f t="shared" si="9"/>
-        <v>325.97663389858718</v>
+        <f>5.67*10^-8*(C143+$E$2+273.14)^4</f>
+        <v>325.88193862809806</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
@@ -7549,15 +7544,15 @@
         <v>0.89</v>
       </c>
       <c r="C144">
-        <v>2.21</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="D144">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B144+$E$1+273.14)^4</f>
         <v>390.24195308984537</v>
       </c>
       <c r="E144">
-        <f t="shared" si="9"/>
-        <v>325.92928368402693</v>
+        <f>5.67*10^-8*(C144+$E$2+273.14)^4</f>
+        <v>325.78726399063476</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
@@ -7568,15 +7563,15 @@
         <v>1.02</v>
       </c>
       <c r="C145">
-        <v>3.65</v>
+        <v>3.66</v>
       </c>
       <c r="D145">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B145+$E$1+273.14)^4</f>
         <v>390.94696034716645</v>
       </c>
       <c r="E145">
-        <f t="shared" si="9"/>
-        <v>332.80101455345243</v>
+        <f>5.67*10^-8*(C145+$E$2+273.14)^4</f>
+        <v>332.84911152955391</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
@@ -7590,11 +7585,11 @@
         <v>2.7</v>
       </c>
       <c r="D146">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B146+$E$1+273.14)^4</f>
         <v>390.4045623706611</v>
       </c>
       <c r="E146">
-        <f t="shared" si="9"/>
+        <f>5.67*10^-8*(C146+$E$2+273.14)^4</f>
         <v>328.25551809487763</v>
       </c>
     </row>
@@ -7606,15 +7601,15 @@
         <v>0.85</v>
       </c>
       <c r="C147">
-        <v>2.42</v>
+        <v>2.4</v>
       </c>
       <c r="D147">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B147+$E$1+273.14)^4</f>
         <v>390.02521973919369</v>
       </c>
       <c r="E147">
-        <f t="shared" si="9"/>
-        <v>326.92472207944598</v>
+        <f>5.67*10^-8*(C147+$E$2+273.14)^4</f>
+        <v>326.82982031380078</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
@@ -7622,18 +7617,18 @@
         <v>2019</v>
       </c>
       <c r="B148">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="C148">
-        <v>2.91</v>
+        <v>2.84</v>
       </c>
       <c r="D148">
-        <f t="shared" si="8"/>
-        <v>390.72993338113662</v>
+        <f>5.67*10^-8*(B148+$E$1+273.14)^4</f>
+        <v>390.67569076114364</v>
       </c>
       <c r="E148">
-        <f t="shared" si="9"/>
-        <v>329.25627822655298</v>
+        <f>5.67*10^-8*(C148+$E$2+273.14)^4</f>
+        <v>328.92243762799313</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
@@ -7641,18 +7636,18 @@
         <v>2020</v>
       </c>
       <c r="B149">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="C149">
-        <v>3.1</v>
+        <v>3.15</v>
       </c>
       <c r="D149">
-        <f t="shared" si="8"/>
-        <v>390.89269513196621</v>
+        <f>5.67*10^-8*(B149+$E$1+273.14)^4</f>
+        <v>390.94696034716645</v>
       </c>
       <c r="E149">
-        <f t="shared" si="9"/>
-        <v>330.16369803388989</v>
+        <f>5.67*10^-8*(C149+$E$2+273.14)^4</f>
+        <v>330.4028041367705</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
@@ -7663,72 +7658,15 @@
         <v>0.85</v>
       </c>
       <c r="C150">
-        <v>2.4500000000000002</v>
+        <v>2.42</v>
       </c>
       <c r="D150">
-        <f t="shared" si="8"/>
+        <f>5.67*10^-8*(B150+$E$1+273.14)^4</f>
         <v>390.02521973919369</v>
       </c>
       <c r="E150">
-        <f t="shared" si="9"/>
-        <v>327.06711347762115</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151">
-        <v>2022</v>
-      </c>
-      <c r="B151">
-        <v>0.9</v>
-      </c>
-      <c r="C151">
-        <v>2.54</v>
-      </c>
-      <c r="D151">
-        <f t="shared" si="8"/>
-        <v>390.29615053824244</v>
-      </c>
-      <c r="E151">
-        <f t="shared" si="9"/>
-        <v>327.49456676454707</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152">
-        <v>2023</v>
-      </c>
-      <c r="B152">
-        <v>1.17</v>
-      </c>
-      <c r="C152">
-        <v>2.79</v>
-      </c>
-      <c r="D152">
-        <f t="shared" si="8"/>
-        <v>391.76161676863984</v>
-      </c>
-      <c r="E152">
-        <f t="shared" si="9"/>
-        <v>328.68413553302315</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153">
-        <v>2024</v>
-      </c>
-      <c r="B153">
-        <v>1.29</v>
-      </c>
-      <c r="C153">
-        <v>3.15</v>
-      </c>
-      <c r="D153">
-        <f t="shared" si="8"/>
-        <v>392.4142580601096</v>
-      </c>
-      <c r="E153">
-        <f t="shared" si="9"/>
-        <v>330.4028041367705</v>
+        <f>5.67*10^-8*(C150+$E$2+273.14)^4</f>
+        <v>326.92472207944598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>